<commit_message>
Update Excel template names
</commit_message>
<xml_diff>
--- a/public/data/Master App Timesheet.xlsx
+++ b/public/data/Master App Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgelD\timesheet-app\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56F6D55-9E7A-4264-B4DB-1E0256167DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03989A7-30A1-494C-BD18-814BE3503E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendor Entry Sheet" sheetId="5" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2891" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2896" uniqueCount="662">
   <si>
     <t xml:space="preserve">Date
 </t>
@@ -2093,7 +2093,7 @@
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
     <numFmt numFmtId="165" formatCode="0000"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2293,17 +2293,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2763,7 +2752,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2935,12 +2924,6 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2952,9 +2935,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2982,24 +2962,6 @@
     <xf numFmtId="0" fontId="26" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -3522,14 +3484,14 @@
     <row r="1" spans="1:15" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13"/>
       <c r="B1" s="13"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
       <c r="G1" s="49"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
       <c r="K1" s="13"/>
       <c r="M1" s="45"/>
       <c r="N1" s="46"/>
@@ -3613,14 +3575,14 @@
       <c r="A4" s="51"/>
       <c r="B4" s="32"/>
       <c r="C4" s="33"/>
-      <c r="D4" s="58"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="34"/>
       <c r="F4" s="36"/>
       <c r="G4" s="33"/>
       <c r="H4" s="37"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="60"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="58"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="51"/>
@@ -3629,7 +3591,7 @@
         <f>IFERROR(VLOOKUP(B5,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D5" s="58" t="str">
+      <c r="D5" s="56" t="str">
         <f>IFERROR(VLOOKUP(B5,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -3637,15 +3599,15 @@
       <c r="F5" s="36"/>
       <c r="G5" s="33"/>
       <c r="H5" s="37"/>
-      <c r="I5" s="59" t="str">
+      <c r="I5" s="57" t="str">
         <f>IF(B5="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J5" s="59" t="str">
+      <c r="J5" s="57" t="str">
         <f>IF(B5="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K5" s="60" t="str">
+      <c r="K5" s="58" t="str">
         <f>IFERROR(VLOOKUP(B5,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -3657,7 +3619,7 @@
         <f>IFERROR(VLOOKUP(B6,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D6" s="58" t="str">
+      <c r="D6" s="56" t="str">
         <f>IFERROR(VLOOKUP(B6,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -3665,15 +3627,15 @@
       <c r="F6" s="36"/>
       <c r="G6" s="33"/>
       <c r="H6" s="37"/>
-      <c r="I6" s="59" t="str">
+      <c r="I6" s="57" t="str">
         <f>IF(B6="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J6" s="59" t="str">
+      <c r="J6" s="57" t="str">
         <f>IF(B6="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K6" s="60" t="str">
+      <c r="K6" s="58" t="str">
         <f>IFERROR(VLOOKUP(B6,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -3685,7 +3647,7 @@
         <f>IFERROR(VLOOKUP(B7,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D7" s="58" t="str">
+      <c r="D7" s="56" t="str">
         <f>IFERROR(VLOOKUP(B7,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -3693,15 +3655,15 @@
       <c r="F7" s="36"/>
       <c r="G7" s="33"/>
       <c r="H7" s="37"/>
-      <c r="I7" s="59" t="str">
+      <c r="I7" s="57" t="str">
         <f>IF(B7="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J7" s="59" t="str">
+      <c r="J7" s="57" t="str">
         <f>IF(B7="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K7" s="60" t="str">
+      <c r="K7" s="58" t="str">
         <f>IFERROR(VLOOKUP(B7,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -3713,7 +3675,7 @@
         <f>IFERROR(VLOOKUP(B8,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D8" s="58" t="str">
+      <c r="D8" s="56" t="str">
         <f>IFERROR(VLOOKUP(B8,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -3721,15 +3683,15 @@
       <c r="F8" s="36"/>
       <c r="G8" s="33"/>
       <c r="H8" s="37"/>
-      <c r="I8" s="59" t="str">
+      <c r="I8" s="57" t="str">
         <f>IF(B8="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J8" s="59" t="str">
+      <c r="J8" s="57" t="str">
         <f>IF(B8="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K8" s="60" t="str">
+      <c r="K8" s="58" t="str">
         <f>IFERROR(VLOOKUP(B8,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -3741,7 +3703,7 @@
         <f>IFERROR(VLOOKUP(B9,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D9" s="58" t="str">
+      <c r="D9" s="56" t="str">
         <f>IFERROR(VLOOKUP(B9,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -3749,15 +3711,15 @@
       <c r="F9" s="36"/>
       <c r="G9" s="33"/>
       <c r="H9" s="37"/>
-      <c r="I9" s="59" t="str">
+      <c r="I9" s="57" t="str">
         <f>IF(B9="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J9" s="59" t="str">
+      <c r="J9" s="57" t="str">
         <f>IF(B9="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K9" s="60" t="str">
+      <c r="K9" s="58" t="str">
         <f>IFERROR(VLOOKUP(B9,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -3769,7 +3731,7 @@
         <f>IFERROR(VLOOKUP(B10,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D10" s="58" t="str">
+      <c r="D10" s="56" t="str">
         <f>IFERROR(VLOOKUP(B10,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -3777,15 +3739,15 @@
       <c r="F10" s="36"/>
       <c r="G10" s="33"/>
       <c r="H10" s="37"/>
-      <c r="I10" s="59" t="str">
+      <c r="I10" s="57" t="str">
         <f>IF(B10="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J10" s="59" t="str">
+      <c r="J10" s="57" t="str">
         <f>IF(B10="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K10" s="60" t="str">
+      <c r="K10" s="58" t="str">
         <f>IFERROR(VLOOKUP(B10,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -3797,7 +3759,7 @@
         <f>IFERROR(VLOOKUP(B11,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D11" s="58" t="str">
+      <c r="D11" s="56" t="str">
         <f>IFERROR(VLOOKUP(B11,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -3805,15 +3767,15 @@
       <c r="F11" s="36"/>
       <c r="G11" s="33"/>
       <c r="H11" s="37"/>
-      <c r="I11" s="59" t="str">
+      <c r="I11" s="57" t="str">
         <f>IF(B11="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J11" s="59" t="str">
+      <c r="J11" s="57" t="str">
         <f>IF(B11="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K11" s="60" t="str">
+      <c r="K11" s="58" t="str">
         <f>IFERROR(VLOOKUP(B11,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -3825,7 +3787,7 @@
         <f>IFERROR(VLOOKUP(B12,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D12" s="58" t="str">
+      <c r="D12" s="56" t="str">
         <f>IFERROR(VLOOKUP(B12,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -3833,15 +3795,15 @@
       <c r="F12" s="36"/>
       <c r="G12" s="33"/>
       <c r="H12" s="37"/>
-      <c r="I12" s="59" t="str">
+      <c r="I12" s="57" t="str">
         <f>IF(B12="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J12" s="59" t="str">
+      <c r="J12" s="57" t="str">
         <f>IF(B12="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K12" s="60" t="str">
+      <c r="K12" s="58" t="str">
         <f>IFERROR(VLOOKUP(B12,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -3853,7 +3815,7 @@
         <f>IFERROR(VLOOKUP(B13,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D13" s="58" t="str">
+      <c r="D13" s="56" t="str">
         <f>IFERROR(VLOOKUP(B13,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -3861,15 +3823,15 @@
       <c r="F13" s="36"/>
       <c r="G13" s="33"/>
       <c r="H13" s="37"/>
-      <c r="I13" s="59" t="str">
+      <c r="I13" s="57" t="str">
         <f>IF(B13="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J13" s="59" t="str">
+      <c r="J13" s="57" t="str">
         <f>IF(B13="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K13" s="60" t="str">
+      <c r="K13" s="58" t="str">
         <f>IFERROR(VLOOKUP(B13,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -3881,7 +3843,7 @@
         <f>IFERROR(VLOOKUP(B14,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D14" s="58" t="str">
+      <c r="D14" s="56" t="str">
         <f>IFERROR(VLOOKUP(B14,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -3889,15 +3851,15 @@
       <c r="F14" s="36"/>
       <c r="G14" s="33"/>
       <c r="H14" s="37"/>
-      <c r="I14" s="59" t="str">
+      <c r="I14" s="57" t="str">
         <f>IF(B14="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J14" s="59" t="str">
+      <c r="J14" s="57" t="str">
         <f>IF(B14="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K14" s="60" t="str">
+      <c r="K14" s="58" t="str">
         <f>IFERROR(VLOOKUP(B14,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -3909,7 +3871,7 @@
         <f>IFERROR(VLOOKUP(B15,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D15" s="58" t="str">
+      <c r="D15" s="56" t="str">
         <f>IFERROR(VLOOKUP(B15,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -3917,15 +3879,15 @@
       <c r="F15" s="36"/>
       <c r="G15" s="33"/>
       <c r="H15" s="37"/>
-      <c r="I15" s="59" t="str">
+      <c r="I15" s="57" t="str">
         <f>IF(B15="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J15" s="59" t="str">
+      <c r="J15" s="57" t="str">
         <f>IF(B15="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K15" s="60" t="str">
+      <c r="K15" s="58" t="str">
         <f>IFERROR(VLOOKUP(B15,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -3937,7 +3899,7 @@
         <f>IFERROR(VLOOKUP(B16,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D16" s="58" t="str">
+      <c r="D16" s="56" t="str">
         <f>IFERROR(VLOOKUP(B16,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -3945,15 +3907,15 @@
       <c r="F16" s="36"/>
       <c r="G16" s="33"/>
       <c r="H16" s="37"/>
-      <c r="I16" s="59" t="str">
+      <c r="I16" s="57" t="str">
         <f>IF(B16="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J16" s="59" t="str">
+      <c r="J16" s="57" t="str">
         <f>IF(B16="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K16" s="60" t="str">
+      <c r="K16" s="58" t="str">
         <f>IFERROR(VLOOKUP(B16,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -3965,7 +3927,7 @@
         <f>IFERROR(VLOOKUP(B17,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D17" s="58" t="str">
+      <c r="D17" s="56" t="str">
         <f>IFERROR(VLOOKUP(B17,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -3973,15 +3935,15 @@
       <c r="F17" s="36"/>
       <c r="G17" s="33"/>
       <c r="H17" s="37"/>
-      <c r="I17" s="59" t="str">
+      <c r="I17" s="57" t="str">
         <f>IF(B17="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J17" s="59" t="str">
+      <c r="J17" s="57" t="str">
         <f>IF(B17="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K17" s="60" t="str">
+      <c r="K17" s="58" t="str">
         <f>IFERROR(VLOOKUP(B17,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -3993,7 +3955,7 @@
         <f>IFERROR(VLOOKUP(B18,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D18" s="58" t="str">
+      <c r="D18" s="56" t="str">
         <f>IFERROR(VLOOKUP(B18,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4001,15 +3963,15 @@
       <c r="F18" s="36"/>
       <c r="G18" s="33"/>
       <c r="H18" s="37"/>
-      <c r="I18" s="59" t="str">
+      <c r="I18" s="57" t="str">
         <f>IF(B18="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J18" s="59" t="str">
+      <c r="J18" s="57" t="str">
         <f>IF(B18="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K18" s="60" t="str">
+      <c r="K18" s="58" t="str">
         <f>IFERROR(VLOOKUP(B18,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4021,7 +3983,7 @@
         <f>IFERROR(VLOOKUP(B19,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D19" s="58" t="str">
+      <c r="D19" s="56" t="str">
         <f>IFERROR(VLOOKUP(B19,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4029,15 +3991,15 @@
       <c r="F19" s="36"/>
       <c r="G19" s="33"/>
       <c r="H19" s="37"/>
-      <c r="I19" s="59" t="str">
+      <c r="I19" s="57" t="str">
         <f>IF(B19="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J19" s="59" t="str">
+      <c r="J19" s="57" t="str">
         <f>IF(B19="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K19" s="60" t="str">
+      <c r="K19" s="58" t="str">
         <f>IFERROR(VLOOKUP(B19,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4049,7 +4011,7 @@
         <f>IFERROR(VLOOKUP(B20,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D20" s="58" t="str">
+      <c r="D20" s="56" t="str">
         <f>IFERROR(VLOOKUP(B20,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4057,15 +4019,15 @@
       <c r="F20" s="36"/>
       <c r="G20" s="33"/>
       <c r="H20" s="37"/>
-      <c r="I20" s="59" t="str">
+      <c r="I20" s="57" t="str">
         <f>IF(B20="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J20" s="59" t="str">
+      <c r="J20" s="57" t="str">
         <f>IF(B20="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K20" s="60" t="str">
+      <c r="K20" s="58" t="str">
         <f>IFERROR(VLOOKUP(B20,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4077,7 +4039,7 @@
         <f>IFERROR(VLOOKUP(B21,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D21" s="58" t="str">
+      <c r="D21" s="56" t="str">
         <f>IFERROR(VLOOKUP(B21,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4085,15 +4047,15 @@
       <c r="F21" s="36"/>
       <c r="G21" s="33"/>
       <c r="H21" s="37"/>
-      <c r="I21" s="59" t="str">
+      <c r="I21" s="57" t="str">
         <f>IF(B21="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J21" s="59" t="str">
+      <c r="J21" s="57" t="str">
         <f>IF(B21="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K21" s="60" t="str">
+      <c r="K21" s="58" t="str">
         <f>IFERROR(VLOOKUP(B21,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4105,7 +4067,7 @@
         <f>IFERROR(VLOOKUP(B22,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D22" s="58" t="str">
+      <c r="D22" s="56" t="str">
         <f>IFERROR(VLOOKUP(B22,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4113,15 +4075,15 @@
       <c r="F22" s="36"/>
       <c r="G22" s="33"/>
       <c r="H22" s="37"/>
-      <c r="I22" s="59" t="str">
+      <c r="I22" s="57" t="str">
         <f>IF(B22="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J22" s="59" t="str">
+      <c r="J22" s="57" t="str">
         <f>IF(B22="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K22" s="60" t="str">
+      <c r="K22" s="58" t="str">
         <f>IFERROR(VLOOKUP(B22,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4133,7 +4095,7 @@
         <f>IFERROR(VLOOKUP(B23,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D23" s="58" t="str">
+      <c r="D23" s="56" t="str">
         <f>IFERROR(VLOOKUP(B23,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4141,15 +4103,15 @@
       <c r="F23" s="36"/>
       <c r="G23" s="33"/>
       <c r="H23" s="37"/>
-      <c r="I23" s="59" t="str">
+      <c r="I23" s="57" t="str">
         <f>IF(B23="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J23" s="59" t="str">
+      <c r="J23" s="57" t="str">
         <f>IF(B23="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K23" s="60" t="str">
+      <c r="K23" s="58" t="str">
         <f>IFERROR(VLOOKUP(B23,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4161,7 +4123,7 @@
         <f>IFERROR(VLOOKUP(B24,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D24" s="58" t="str">
+      <c r="D24" s="56" t="str">
         <f>IFERROR(VLOOKUP(B24,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4169,15 +4131,15 @@
       <c r="F24" s="36"/>
       <c r="G24" s="33"/>
       <c r="H24" s="37"/>
-      <c r="I24" s="59" t="str">
+      <c r="I24" s="57" t="str">
         <f>IF(B24="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J24" s="59" t="str">
+      <c r="J24" s="57" t="str">
         <f>IF(B24="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K24" s="60" t="str">
+      <c r="K24" s="58" t="str">
         <f>IFERROR(VLOOKUP(B24,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4189,7 +4151,7 @@
         <f>IFERROR(VLOOKUP(B25,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D25" s="58" t="str">
+      <c r="D25" s="56" t="str">
         <f>IFERROR(VLOOKUP(B25,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4197,15 +4159,15 @@
       <c r="F25" s="36"/>
       <c r="G25" s="33"/>
       <c r="H25" s="37"/>
-      <c r="I25" s="59" t="str">
+      <c r="I25" s="57" t="str">
         <f>IF(B25="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J25" s="59" t="str">
+      <c r="J25" s="57" t="str">
         <f>IF(B25="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K25" s="60" t="str">
+      <c r="K25" s="58" t="str">
         <f>IFERROR(VLOOKUP(B25,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4217,7 +4179,7 @@
         <f>IFERROR(VLOOKUP(B26,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D26" s="58" t="str">
+      <c r="D26" s="56" t="str">
         <f>IFERROR(VLOOKUP(B26,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4225,15 +4187,15 @@
       <c r="F26" s="36"/>
       <c r="G26" s="33"/>
       <c r="H26" s="37"/>
-      <c r="I26" s="59" t="str">
+      <c r="I26" s="57" t="str">
         <f>IF(B26="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J26" s="59" t="str">
+      <c r="J26" s="57" t="str">
         <f>IF(B26="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K26" s="60" t="str">
+      <c r="K26" s="58" t="str">
         <f>IFERROR(VLOOKUP(B26,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4245,7 +4207,7 @@
         <f>IFERROR(VLOOKUP(B27,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D27" s="58" t="str">
+      <c r="D27" s="56" t="str">
         <f>IFERROR(VLOOKUP(B27,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4253,15 +4215,15 @@
       <c r="F27" s="36"/>
       <c r="G27" s="33"/>
       <c r="H27" s="37"/>
-      <c r="I27" s="59" t="str">
+      <c r="I27" s="57" t="str">
         <f>IF(B27="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J27" s="59" t="str">
+      <c r="J27" s="57" t="str">
         <f>IF(B27="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K27" s="60" t="str">
+      <c r="K27" s="58" t="str">
         <f>IFERROR(VLOOKUP(B27,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4273,7 +4235,7 @@
         <f>IFERROR(VLOOKUP(B28,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D28" s="58" t="str">
+      <c r="D28" s="56" t="str">
         <f>IFERROR(VLOOKUP(B28,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4281,15 +4243,15 @@
       <c r="F28" s="36"/>
       <c r="G28" s="33"/>
       <c r="H28" s="37"/>
-      <c r="I28" s="59" t="str">
+      <c r="I28" s="57" t="str">
         <f>IF(B28="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J28" s="59" t="str">
+      <c r="J28" s="57" t="str">
         <f>IF(B28="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K28" s="60" t="str">
+      <c r="K28" s="58" t="str">
         <f>IFERROR(VLOOKUP(B28,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4301,7 +4263,7 @@
         <f>IFERROR(VLOOKUP(B29,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D29" s="58" t="str">
+      <c r="D29" s="56" t="str">
         <f>IFERROR(VLOOKUP(B29,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4309,15 +4271,15 @@
       <c r="F29" s="36"/>
       <c r="G29" s="33"/>
       <c r="H29" s="37"/>
-      <c r="I29" s="59" t="str">
+      <c r="I29" s="57" t="str">
         <f>IF(B29="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J29" s="59" t="str">
+      <c r="J29" s="57" t="str">
         <f>IF(B29="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K29" s="60" t="str">
+      <c r="K29" s="58" t="str">
         <f>IFERROR(VLOOKUP(B29,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4329,7 +4291,7 @@
         <f>IFERROR(VLOOKUP(B30,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D30" s="58" t="str">
+      <c r="D30" s="56" t="str">
         <f>IFERROR(VLOOKUP(B30,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4337,15 +4299,15 @@
       <c r="F30" s="36"/>
       <c r="G30" s="33"/>
       <c r="H30" s="37"/>
-      <c r="I30" s="59" t="str">
+      <c r="I30" s="57" t="str">
         <f>IF(B30="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J30" s="59" t="str">
+      <c r="J30" s="57" t="str">
         <f>IF(B30="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K30" s="60" t="str">
+      <c r="K30" s="58" t="str">
         <f>IFERROR(VLOOKUP(B30,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4357,7 +4319,7 @@
         <f>IFERROR(VLOOKUP(B31,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D31" s="58" t="str">
+      <c r="D31" s="56" t="str">
         <f>IFERROR(VLOOKUP(B31,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4365,15 +4327,15 @@
       <c r="F31" s="36"/>
       <c r="G31" s="33"/>
       <c r="H31" s="37"/>
-      <c r="I31" s="59" t="str">
+      <c r="I31" s="57" t="str">
         <f>IF(B31="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J31" s="59" t="str">
+      <c r="J31" s="57" t="str">
         <f>IF(B31="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K31" s="60" t="str">
+      <c r="K31" s="58" t="str">
         <f>IFERROR(VLOOKUP(B31,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4385,7 +4347,7 @@
         <f>IFERROR(VLOOKUP(B32,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D32" s="58" t="str">
+      <c r="D32" s="56" t="str">
         <f>IFERROR(VLOOKUP(B32,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4393,15 +4355,15 @@
       <c r="F32" s="36"/>
       <c r="G32" s="33"/>
       <c r="H32" s="37"/>
-      <c r="I32" s="59" t="str">
+      <c r="I32" s="57" t="str">
         <f>IF(B32="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J32" s="59" t="str">
+      <c r="J32" s="57" t="str">
         <f>IF(B32="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K32" s="60" t="str">
+      <c r="K32" s="58" t="str">
         <f>IFERROR(VLOOKUP(B32,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4413,7 +4375,7 @@
         <f>IFERROR(VLOOKUP(B33,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D33" s="58" t="str">
+      <c r="D33" s="56" t="str">
         <f>IFERROR(VLOOKUP(B33,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4421,15 +4383,15 @@
       <c r="F33" s="36"/>
       <c r="G33" s="33"/>
       <c r="H33" s="37"/>
-      <c r="I33" s="59" t="str">
+      <c r="I33" s="57" t="str">
         <f>IF(B33="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J33" s="59" t="str">
+      <c r="J33" s="57" t="str">
         <f>IF(B33="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K33" s="60" t="str">
+      <c r="K33" s="58" t="str">
         <f>IFERROR(VLOOKUP(B33,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4441,7 +4403,7 @@
         <f>IFERROR(VLOOKUP(B34,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D34" s="58" t="str">
+      <c r="D34" s="56" t="str">
         <f>IFERROR(VLOOKUP(B34,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4449,15 +4411,15 @@
       <c r="F34" s="36"/>
       <c r="G34" s="33"/>
       <c r="H34" s="37"/>
-      <c r="I34" s="59" t="str">
+      <c r="I34" s="57" t="str">
         <f>IF(B34="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J34" s="59" t="str">
+      <c r="J34" s="57" t="str">
         <f>IF(B34="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K34" s="60" t="str">
+      <c r="K34" s="58" t="str">
         <f>IFERROR(VLOOKUP(B34,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4469,7 +4431,7 @@
         <f>IFERROR(VLOOKUP(B35,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D35" s="58" t="str">
+      <c r="D35" s="56" t="str">
         <f>IFERROR(VLOOKUP(B35,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4477,15 +4439,15 @@
       <c r="F35" s="36"/>
       <c r="G35" s="33"/>
       <c r="H35" s="37"/>
-      <c r="I35" s="59" t="str">
+      <c r="I35" s="57" t="str">
         <f>IF(B35="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J35" s="59" t="str">
+      <c r="J35" s="57" t="str">
         <f>IF(B35="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K35" s="60" t="str">
+      <c r="K35" s="58" t="str">
         <f>IFERROR(VLOOKUP(B35,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4497,7 +4459,7 @@
         <f>IFERROR(VLOOKUP(B36,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D36" s="58" t="str">
+      <c r="D36" s="56" t="str">
         <f>IFERROR(VLOOKUP(B36,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4505,15 +4467,15 @@
       <c r="F36" s="36"/>
       <c r="G36" s="33"/>
       <c r="H36" s="37"/>
-      <c r="I36" s="59" t="str">
+      <c r="I36" s="57" t="str">
         <f>IF(B36="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J36" s="59" t="str">
+      <c r="J36" s="57" t="str">
         <f>IF(B36="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K36" s="60" t="str">
+      <c r="K36" s="58" t="str">
         <f>IFERROR(VLOOKUP(B36,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4525,7 +4487,7 @@
         <f>IFERROR(VLOOKUP(B37,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D37" s="58" t="str">
+      <c r="D37" s="56" t="str">
         <f>IFERROR(VLOOKUP(B37,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4533,15 +4495,15 @@
       <c r="F37" s="36"/>
       <c r="G37" s="33"/>
       <c r="H37" s="37"/>
-      <c r="I37" s="59" t="str">
+      <c r="I37" s="57" t="str">
         <f>IF(B37="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J37" s="59" t="str">
+      <c r="J37" s="57" t="str">
         <f>IF(B37="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K37" s="60" t="str">
+      <c r="K37" s="58" t="str">
         <f>IFERROR(VLOOKUP(B37,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4553,7 +4515,7 @@
         <f>IFERROR(VLOOKUP(B38,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D38" s="58" t="str">
+      <c r="D38" s="56" t="str">
         <f>IFERROR(VLOOKUP(B38,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4561,15 +4523,15 @@
       <c r="F38" s="36"/>
       <c r="G38" s="33"/>
       <c r="H38" s="37"/>
-      <c r="I38" s="59" t="str">
+      <c r="I38" s="57" t="str">
         <f>IF(B38="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J38" s="59" t="str">
+      <c r="J38" s="57" t="str">
         <f>IF(B38="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K38" s="60" t="str">
+      <c r="K38" s="58" t="str">
         <f>IFERROR(VLOOKUP(B38,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4581,7 +4543,7 @@
         <f>IFERROR(VLOOKUP(B39,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D39" s="58" t="str">
+      <c r="D39" s="56" t="str">
         <f>IFERROR(VLOOKUP(B39,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4589,15 +4551,15 @@
       <c r="F39" s="36"/>
       <c r="G39" s="33"/>
       <c r="H39" s="37"/>
-      <c r="I39" s="59" t="str">
+      <c r="I39" s="57" t="str">
         <f>IF(B39="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J39" s="59" t="str">
+      <c r="J39" s="57" t="str">
         <f>IF(B39="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K39" s="60" t="str">
+      <c r="K39" s="58" t="str">
         <f>IFERROR(VLOOKUP(B39,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4609,7 +4571,7 @@
         <f>IFERROR(VLOOKUP(B40,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D40" s="58" t="str">
+      <c r="D40" s="56" t="str">
         <f>IFERROR(VLOOKUP(B40,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4617,15 +4579,15 @@
       <c r="F40" s="36"/>
       <c r="G40" s="33"/>
       <c r="H40" s="37"/>
-      <c r="I40" s="59" t="str">
+      <c r="I40" s="57" t="str">
         <f>IF(B40="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J40" s="59" t="str">
+      <c r="J40" s="57" t="str">
         <f>IF(B40="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K40" s="60" t="str">
+      <c r="K40" s="58" t="str">
         <f>IFERROR(VLOOKUP(B40,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4637,7 +4599,7 @@
         <f>IFERROR(VLOOKUP(B41,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D41" s="58" t="str">
+      <c r="D41" s="56" t="str">
         <f>IFERROR(VLOOKUP(B41,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4645,15 +4607,15 @@
       <c r="F41" s="36"/>
       <c r="G41" s="33"/>
       <c r="H41" s="37"/>
-      <c r="I41" s="59" t="str">
+      <c r="I41" s="57" t="str">
         <f>IF(B41="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J41" s="59" t="str">
+      <c r="J41" s="57" t="str">
         <f>IF(B41="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K41" s="60" t="str">
+      <c r="K41" s="58" t="str">
         <f>IFERROR(VLOOKUP(B41,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4665,7 +4627,7 @@
         <f>IFERROR(VLOOKUP(B42,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D42" s="58" t="str">
+      <c r="D42" s="56" t="str">
         <f>IFERROR(VLOOKUP(B42,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4673,15 +4635,15 @@
       <c r="F42" s="36"/>
       <c r="G42" s="33"/>
       <c r="H42" s="37"/>
-      <c r="I42" s="59" t="str">
+      <c r="I42" s="57" t="str">
         <f>IF(B42="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J42" s="59" t="str">
+      <c r="J42" s="57" t="str">
         <f>IF(B42="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K42" s="60" t="str">
+      <c r="K42" s="58" t="str">
         <f>IFERROR(VLOOKUP(B42,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4693,7 +4655,7 @@
         <f>IFERROR(VLOOKUP(B43,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D43" s="58" t="str">
+      <c r="D43" s="56" t="str">
         <f>IFERROR(VLOOKUP(B43,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4701,15 +4663,15 @@
       <c r="F43" s="36"/>
       <c r="G43" s="33"/>
       <c r="H43" s="37"/>
-      <c r="I43" s="59" t="str">
+      <c r="I43" s="57" t="str">
         <f>IF(B43="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J43" s="59" t="str">
+      <c r="J43" s="57" t="str">
         <f>IF(B43="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K43" s="60" t="str">
+      <c r="K43" s="58" t="str">
         <f>IFERROR(VLOOKUP(B43,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4721,7 +4683,7 @@
         <f>IFERROR(VLOOKUP(B44,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D44" s="58" t="str">
+      <c r="D44" s="56" t="str">
         <f>IFERROR(VLOOKUP(B44,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4729,15 +4691,15 @@
       <c r="F44" s="36"/>
       <c r="G44" s="33"/>
       <c r="H44" s="37"/>
-      <c r="I44" s="59" t="str">
+      <c r="I44" s="57" t="str">
         <f>IF(B44="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J44" s="59" t="str">
+      <c r="J44" s="57" t="str">
         <f>IF(B44="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K44" s="60" t="str">
+      <c r="K44" s="58" t="str">
         <f>IFERROR(VLOOKUP(B44,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4749,7 +4711,7 @@
         <f>IFERROR(VLOOKUP(B45,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D45" s="58" t="str">
+      <c r="D45" s="56" t="str">
         <f>IFERROR(VLOOKUP(B45,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4757,15 +4719,15 @@
       <c r="F45" s="36"/>
       <c r="G45" s="33"/>
       <c r="H45" s="37"/>
-      <c r="I45" s="59" t="str">
+      <c r="I45" s="57" t="str">
         <f>IF(B45="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J45" s="59" t="str">
+      <c r="J45" s="57" t="str">
         <f>IF(B45="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K45" s="60" t="str">
+      <c r="K45" s="58" t="str">
         <f>IFERROR(VLOOKUP(B45,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4777,7 +4739,7 @@
         <f>IFERROR(VLOOKUP(B46,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D46" s="58" t="str">
+      <c r="D46" s="56" t="str">
         <f>IFERROR(VLOOKUP(B46,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4785,15 +4747,15 @@
       <c r="F46" s="36"/>
       <c r="G46" s="33"/>
       <c r="H46" s="37"/>
-      <c r="I46" s="59" t="str">
+      <c r="I46" s="57" t="str">
         <f>IF(B46="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J46" s="59" t="str">
+      <c r="J46" s="57" t="str">
         <f>IF(B46="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K46" s="60" t="str">
+      <c r="K46" s="58" t="str">
         <f>IFERROR(VLOOKUP(B46,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4805,7 +4767,7 @@
         <f>IFERROR(VLOOKUP(B47,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D47" s="58" t="str">
+      <c r="D47" s="56" t="str">
         <f>IFERROR(VLOOKUP(B47,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4813,15 +4775,15 @@
       <c r="F47" s="36"/>
       <c r="G47" s="33"/>
       <c r="H47" s="37"/>
-      <c r="I47" s="59" t="str">
+      <c r="I47" s="57" t="str">
         <f>IF(B47="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J47" s="59" t="str">
+      <c r="J47" s="57" t="str">
         <f>IF(B47="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K47" s="60" t="str">
+      <c r="K47" s="58" t="str">
         <f>IFERROR(VLOOKUP(B47,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4833,7 +4795,7 @@
         <f>IFERROR(VLOOKUP(B48,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D48" s="58" t="str">
+      <c r="D48" s="56" t="str">
         <f>IFERROR(VLOOKUP(B48,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4841,15 +4803,15 @@
       <c r="F48" s="36"/>
       <c r="G48" s="33"/>
       <c r="H48" s="37"/>
-      <c r="I48" s="59" t="str">
+      <c r="I48" s="57" t="str">
         <f>IF(B48="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J48" s="59" t="str">
+      <c r="J48" s="57" t="str">
         <f>IF(B48="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K48" s="60" t="str">
+      <c r="K48" s="58" t="str">
         <f>IFERROR(VLOOKUP(B48,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4861,7 +4823,7 @@
         <f>IFERROR(VLOOKUP(B49,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D49" s="58" t="str">
+      <c r="D49" s="56" t="str">
         <f>IFERROR(VLOOKUP(B49,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4869,15 +4831,15 @@
       <c r="F49" s="36"/>
       <c r="G49" s="33"/>
       <c r="H49" s="37"/>
-      <c r="I49" s="59" t="str">
+      <c r="I49" s="57" t="str">
         <f>IF(B49="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J49" s="59" t="str">
+      <c r="J49" s="57" t="str">
         <f>IF(B49="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K49" s="60" t="str">
+      <c r="K49" s="58" t="str">
         <f>IFERROR(VLOOKUP(B49,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4889,7 +4851,7 @@
         <f>IFERROR(VLOOKUP(B50,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D50" s="58" t="str">
+      <c r="D50" s="56" t="str">
         <f>IFERROR(VLOOKUP(B50,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4897,15 +4859,15 @@
       <c r="F50" s="36"/>
       <c r="G50" s="33"/>
       <c r="H50" s="37"/>
-      <c r="I50" s="59" t="str">
+      <c r="I50" s="57" t="str">
         <f>IF(B50="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J50" s="59" t="str">
+      <c r="J50" s="57" t="str">
         <f>IF(B50="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K50" s="60" t="str">
+      <c r="K50" s="58" t="str">
         <f>IFERROR(VLOOKUP(B50,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4917,7 +4879,7 @@
         <f>IFERROR(VLOOKUP(B51,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D51" s="58" t="str">
+      <c r="D51" s="56" t="str">
         <f>IFERROR(VLOOKUP(B51,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4925,15 +4887,15 @@
       <c r="F51" s="36"/>
       <c r="G51" s="33"/>
       <c r="H51" s="37"/>
-      <c r="I51" s="59" t="str">
+      <c r="I51" s="57" t="str">
         <f>IF(B51="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J51" s="59" t="str">
+      <c r="J51" s="57" t="str">
         <f>IF(B51="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K51" s="60" t="str">
+      <c r="K51" s="58" t="str">
         <f>IFERROR(VLOOKUP(B51,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4945,7 +4907,7 @@
         <f>IFERROR(VLOOKUP(B52,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D52" s="58" t="str">
+      <c r="D52" s="56" t="str">
         <f>IFERROR(VLOOKUP(B52,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4953,15 +4915,15 @@
       <c r="F52" s="36"/>
       <c r="G52" s="33"/>
       <c r="H52" s="37"/>
-      <c r="I52" s="59" t="str">
+      <c r="I52" s="57" t="str">
         <f>IF(B52="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J52" s="59" t="str">
+      <c r="J52" s="57" t="str">
         <f>IF(B52="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K52" s="60" t="str">
+      <c r="K52" s="58" t="str">
         <f>IFERROR(VLOOKUP(B52,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -4973,7 +4935,7 @@
         <f>IFERROR(VLOOKUP(B53,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D53" s="58" t="str">
+      <c r="D53" s="56" t="str">
         <f>IFERROR(VLOOKUP(B53,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -4981,15 +4943,15 @@
       <c r="F53" s="36"/>
       <c r="G53" s="33"/>
       <c r="H53" s="37"/>
-      <c r="I53" s="59" t="str">
+      <c r="I53" s="57" t="str">
         <f>IF(B53="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J53" s="59" t="str">
+      <c r="J53" s="57" t="str">
         <f>IF(B53="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K53" s="60" t="str">
+      <c r="K53" s="58" t="str">
         <f>IFERROR(VLOOKUP(B53,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5001,7 +4963,7 @@
         <f>IFERROR(VLOOKUP(B54,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D54" s="58" t="str">
+      <c r="D54" s="56" t="str">
         <f>IFERROR(VLOOKUP(B54,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5009,15 +4971,15 @@
       <c r="F54" s="36"/>
       <c r="G54" s="33"/>
       <c r="H54" s="37"/>
-      <c r="I54" s="59" t="str">
+      <c r="I54" s="57" t="str">
         <f>IF(B54="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J54" s="59" t="str">
+      <c r="J54" s="57" t="str">
         <f>IF(B54="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K54" s="60" t="str">
+      <c r="K54" s="58" t="str">
         <f>IFERROR(VLOOKUP(B54,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5029,7 +4991,7 @@
         <f>IFERROR(VLOOKUP(B55,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D55" s="58" t="str">
+      <c r="D55" s="56" t="str">
         <f>IFERROR(VLOOKUP(B55,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5037,15 +4999,15 @@
       <c r="F55" s="36"/>
       <c r="G55" s="33"/>
       <c r="H55" s="37"/>
-      <c r="I55" s="59" t="str">
+      <c r="I55" s="57" t="str">
         <f>IF(B55="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J55" s="59" t="str">
+      <c r="J55" s="57" t="str">
         <f>IF(B55="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K55" s="60" t="str">
+      <c r="K55" s="58" t="str">
         <f>IFERROR(VLOOKUP(B55,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5057,7 +5019,7 @@
         <f>IFERROR(VLOOKUP(B56,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D56" s="58" t="str">
+      <c r="D56" s="56" t="str">
         <f>IFERROR(VLOOKUP(B56,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5065,15 +5027,15 @@
       <c r="F56" s="36"/>
       <c r="G56" s="33"/>
       <c r="H56" s="37"/>
-      <c r="I56" s="59" t="str">
+      <c r="I56" s="57" t="str">
         <f>IF(B56="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J56" s="59" t="str">
+      <c r="J56" s="57" t="str">
         <f>IF(B56="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K56" s="60" t="str">
+      <c r="K56" s="58" t="str">
         <f>IFERROR(VLOOKUP(B56,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5085,7 +5047,7 @@
         <f>IFERROR(VLOOKUP(B57,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D57" s="58" t="str">
+      <c r="D57" s="56" t="str">
         <f>IFERROR(VLOOKUP(B57,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5093,15 +5055,15 @@
       <c r="F57" s="36"/>
       <c r="G57" s="33"/>
       <c r="H57" s="37"/>
-      <c r="I57" s="59" t="str">
+      <c r="I57" s="57" t="str">
         <f>IF(B57="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J57" s="59" t="str">
+      <c r="J57" s="57" t="str">
         <f>IF(B57="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K57" s="60" t="str">
+      <c r="K57" s="58" t="str">
         <f>IFERROR(VLOOKUP(B57,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5113,7 +5075,7 @@
         <f>IFERROR(VLOOKUP(B58,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D58" s="58" t="str">
+      <c r="D58" s="56" t="str">
         <f>IFERROR(VLOOKUP(B58,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5121,15 +5083,15 @@
       <c r="F58" s="36"/>
       <c r="G58" s="33"/>
       <c r="H58" s="37"/>
-      <c r="I58" s="59" t="str">
+      <c r="I58" s="57" t="str">
         <f>IF(B58="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J58" s="59" t="str">
+      <c r="J58" s="57" t="str">
         <f>IF(B58="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K58" s="60" t="str">
+      <c r="K58" s="58" t="str">
         <f>IFERROR(VLOOKUP(B58,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5141,7 +5103,7 @@
         <f>IFERROR(VLOOKUP(B59,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D59" s="58" t="str">
+      <c r="D59" s="56" t="str">
         <f>IFERROR(VLOOKUP(B59,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5149,15 +5111,15 @@
       <c r="F59" s="36"/>
       <c r="G59" s="33"/>
       <c r="H59" s="37"/>
-      <c r="I59" s="59" t="str">
+      <c r="I59" s="57" t="str">
         <f>IF(B59="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J59" s="59" t="str">
+      <c r="J59" s="57" t="str">
         <f>IF(B59="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K59" s="60" t="str">
+      <c r="K59" s="58" t="str">
         <f>IFERROR(VLOOKUP(B59,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5169,7 +5131,7 @@
         <f>IFERROR(VLOOKUP(B60,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D60" s="58" t="str">
+      <c r="D60" s="56" t="str">
         <f>IFERROR(VLOOKUP(B60,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5177,15 +5139,15 @@
       <c r="F60" s="36"/>
       <c r="G60" s="33"/>
       <c r="H60" s="37"/>
-      <c r="I60" s="59" t="str">
+      <c r="I60" s="57" t="str">
         <f>IF(B60="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J60" s="59" t="str">
+      <c r="J60" s="57" t="str">
         <f>IF(B60="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K60" s="60" t="str">
+      <c r="K60" s="58" t="str">
         <f>IFERROR(VLOOKUP(B60,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5197,7 +5159,7 @@
         <f>IFERROR(VLOOKUP(B61,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D61" s="58" t="str">
+      <c r="D61" s="56" t="str">
         <f>IFERROR(VLOOKUP(B61,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5205,15 +5167,15 @@
       <c r="F61" s="36"/>
       <c r="G61" s="33"/>
       <c r="H61" s="37"/>
-      <c r="I61" s="59" t="str">
+      <c r="I61" s="57" t="str">
         <f>IF(B61="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J61" s="59" t="str">
+      <c r="J61" s="57" t="str">
         <f>IF(B61="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K61" s="60" t="str">
+      <c r="K61" s="58" t="str">
         <f>IFERROR(VLOOKUP(B61,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5225,7 +5187,7 @@
         <f>IFERROR(VLOOKUP(B62,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D62" s="58" t="str">
+      <c r="D62" s="56" t="str">
         <f>IFERROR(VLOOKUP(B62,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5233,15 +5195,15 @@
       <c r="F62" s="36"/>
       <c r="G62" s="33"/>
       <c r="H62" s="37"/>
-      <c r="I62" s="59" t="str">
+      <c r="I62" s="57" t="str">
         <f>IF(B62="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J62" s="59" t="str">
+      <c r="J62" s="57" t="str">
         <f>IF(B62="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K62" s="60" t="str">
+      <c r="K62" s="58" t="str">
         <f>IFERROR(VLOOKUP(B62,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5253,7 +5215,7 @@
         <f>IFERROR(VLOOKUP(B63,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D63" s="58" t="str">
+      <c r="D63" s="56" t="str">
         <f>IFERROR(VLOOKUP(B63,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5261,15 +5223,15 @@
       <c r="F63" s="36"/>
       <c r="G63" s="33"/>
       <c r="H63" s="37"/>
-      <c r="I63" s="59" t="str">
+      <c r="I63" s="57" t="str">
         <f>IF(B63="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J63" s="59" t="str">
+      <c r="J63" s="57" t="str">
         <f>IF(B63="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K63" s="60" t="str">
+      <c r="K63" s="58" t="str">
         <f>IFERROR(VLOOKUP(B63,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5281,7 +5243,7 @@
         <f>IFERROR(VLOOKUP(B64,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D64" s="58" t="str">
+      <c r="D64" s="56" t="str">
         <f>IFERROR(VLOOKUP(B64,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5289,15 +5251,15 @@
       <c r="F64" s="36"/>
       <c r="G64" s="33"/>
       <c r="H64" s="37"/>
-      <c r="I64" s="59" t="str">
+      <c r="I64" s="57" t="str">
         <f>IF(B64="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J64" s="59" t="str">
+      <c r="J64" s="57" t="str">
         <f>IF(B64="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K64" s="60" t="str">
+      <c r="K64" s="58" t="str">
         <f>IFERROR(VLOOKUP(B64,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5309,7 +5271,7 @@
         <f>IFERROR(VLOOKUP(B65,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D65" s="58" t="str">
+      <c r="D65" s="56" t="str">
         <f>IFERROR(VLOOKUP(B65,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5317,15 +5279,15 @@
       <c r="F65" s="36"/>
       <c r="G65" s="33"/>
       <c r="H65" s="37"/>
-      <c r="I65" s="59" t="str">
+      <c r="I65" s="57" t="str">
         <f>IF(B65="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J65" s="59" t="str">
+      <c r="J65" s="57" t="str">
         <f>IF(B65="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K65" s="60" t="str">
+      <c r="K65" s="58" t="str">
         <f>IFERROR(VLOOKUP(B65,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5337,7 +5299,7 @@
         <f>IFERROR(VLOOKUP(B66,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D66" s="58" t="str">
+      <c r="D66" s="56" t="str">
         <f>IFERROR(VLOOKUP(B66,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5345,15 +5307,15 @@
       <c r="F66" s="36"/>
       <c r="G66" s="33"/>
       <c r="H66" s="37"/>
-      <c r="I66" s="59" t="str">
+      <c r="I66" s="57" t="str">
         <f>IF(B66="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J66" s="59" t="str">
+      <c r="J66" s="57" t="str">
         <f>IF(B66="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K66" s="60" t="str">
+      <c r="K66" s="58" t="str">
         <f>IFERROR(VLOOKUP(B66,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5365,7 +5327,7 @@
         <f>IFERROR(VLOOKUP(B67,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D67" s="58" t="str">
+      <c r="D67" s="56" t="str">
         <f>IFERROR(VLOOKUP(B67,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5373,15 +5335,15 @@
       <c r="F67" s="36"/>
       <c r="G67" s="33"/>
       <c r="H67" s="37"/>
-      <c r="I67" s="59" t="str">
+      <c r="I67" s="57" t="str">
         <f>IF(B67="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J67" s="59" t="str">
+      <c r="J67" s="57" t="str">
         <f>IF(B67="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K67" s="60" t="str">
+      <c r="K67" s="58" t="str">
         <f>IFERROR(VLOOKUP(B67,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5393,7 +5355,7 @@
         <f>IFERROR(VLOOKUP(B68,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D68" s="58" t="str">
+      <c r="D68" s="56" t="str">
         <f>IFERROR(VLOOKUP(B68,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5401,15 +5363,15 @@
       <c r="F68" s="36"/>
       <c r="G68" s="33"/>
       <c r="H68" s="37"/>
-      <c r="I68" s="59" t="str">
+      <c r="I68" s="57" t="str">
         <f>IF(B68="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J68" s="59" t="str">
+      <c r="J68" s="57" t="str">
         <f>IF(B68="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K68" s="60" t="str">
+      <c r="K68" s="58" t="str">
         <f>IFERROR(VLOOKUP(B68,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5421,7 +5383,7 @@
         <f>IFERROR(VLOOKUP(B69,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D69" s="58" t="str">
+      <c r="D69" s="56" t="str">
         <f>IFERROR(VLOOKUP(B69,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5429,15 +5391,15 @@
       <c r="F69" s="36"/>
       <c r="G69" s="33"/>
       <c r="H69" s="37"/>
-      <c r="I69" s="59" t="str">
+      <c r="I69" s="57" t="str">
         <f>IF(B69="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J69" s="59" t="str">
+      <c r="J69" s="57" t="str">
         <f>IF(B69="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K69" s="60" t="str">
+      <c r="K69" s="58" t="str">
         <f>IFERROR(VLOOKUP(B69,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5449,7 +5411,7 @@
         <f>IFERROR(VLOOKUP(B70,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D70" s="58" t="str">
+      <c r="D70" s="56" t="str">
         <f>IFERROR(VLOOKUP(B70,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5457,15 +5419,15 @@
       <c r="F70" s="36"/>
       <c r="G70" s="33"/>
       <c r="H70" s="37"/>
-      <c r="I70" s="59" t="str">
+      <c r="I70" s="57" t="str">
         <f>IF(B70="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J70" s="59" t="str">
+      <c r="J70" s="57" t="str">
         <f>IF(B70="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K70" s="60" t="str">
+      <c r="K70" s="58" t="str">
         <f>IFERROR(VLOOKUP(B70,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5477,7 +5439,7 @@
         <f>IFERROR(VLOOKUP(B71,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D71" s="58" t="str">
+      <c r="D71" s="56" t="str">
         <f>IFERROR(VLOOKUP(B71,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5485,15 +5447,15 @@
       <c r="F71" s="36"/>
       <c r="G71" s="33"/>
       <c r="H71" s="37"/>
-      <c r="I71" s="59" t="str">
+      <c r="I71" s="57" t="str">
         <f>IF(B71="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J71" s="59" t="str">
+      <c r="J71" s="57" t="str">
         <f>IF(B71="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K71" s="60" t="str">
+      <c r="K71" s="58" t="str">
         <f>IFERROR(VLOOKUP(B71,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5505,7 +5467,7 @@
         <f>IFERROR(VLOOKUP(B72,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D72" s="58" t="str">
+      <c r="D72" s="56" t="str">
         <f>IFERROR(VLOOKUP(B72,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5513,15 +5475,15 @@
       <c r="F72" s="36"/>
       <c r="G72" s="33"/>
       <c r="H72" s="37"/>
-      <c r="I72" s="59" t="str">
+      <c r="I72" s="57" t="str">
         <f>IF(B72="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J72" s="59" t="str">
+      <c r="J72" s="57" t="str">
         <f>IF(B72="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K72" s="60" t="str">
+      <c r="K72" s="58" t="str">
         <f>IFERROR(VLOOKUP(B72,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5533,7 +5495,7 @@
         <f>IFERROR(VLOOKUP(B73,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D73" s="58" t="str">
+      <c r="D73" s="56" t="str">
         <f>IFERROR(VLOOKUP(B73,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5541,15 +5503,15 @@
       <c r="F73" s="36"/>
       <c r="G73" s="33"/>
       <c r="H73" s="37"/>
-      <c r="I73" s="59" t="str">
+      <c r="I73" s="57" t="str">
         <f>IF(B73="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J73" s="59" t="str">
+      <c r="J73" s="57" t="str">
         <f>IF(B73="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K73" s="60" t="str">
+      <c r="K73" s="58" t="str">
         <f>IFERROR(VLOOKUP(B73,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5561,7 +5523,7 @@
         <f>IFERROR(VLOOKUP(B74,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D74" s="58" t="str">
+      <c r="D74" s="56" t="str">
         <f>IFERROR(VLOOKUP(B74,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5569,15 +5531,15 @@
       <c r="F74" s="36"/>
       <c r="G74" s="33"/>
       <c r="H74" s="37"/>
-      <c r="I74" s="59" t="str">
+      <c r="I74" s="57" t="str">
         <f>IF(B74="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J74" s="59" t="str">
+      <c r="J74" s="57" t="str">
         <f>IF(B74="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K74" s="60" t="str">
+      <c r="K74" s="58" t="str">
         <f>IFERROR(VLOOKUP(B74,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5589,7 +5551,7 @@
         <f>IFERROR(VLOOKUP(B75,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D75" s="58" t="str">
+      <c r="D75" s="56" t="str">
         <f>IFERROR(VLOOKUP(B75,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5597,15 +5559,15 @@
       <c r="F75" s="36"/>
       <c r="G75" s="33"/>
       <c r="H75" s="37"/>
-      <c r="I75" s="59" t="str">
+      <c r="I75" s="57" t="str">
         <f>IF(B75="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J75" s="59" t="str">
+      <c r="J75" s="57" t="str">
         <f>IF(B75="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K75" s="60" t="str">
+      <c r="K75" s="58" t="str">
         <f>IFERROR(VLOOKUP(B75,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5617,7 +5579,7 @@
         <f>IFERROR(VLOOKUP(B76,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D76" s="58" t="str">
+      <c r="D76" s="56" t="str">
         <f>IFERROR(VLOOKUP(B76,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5625,15 +5587,15 @@
       <c r="F76" s="36"/>
       <c r="G76" s="33"/>
       <c r="H76" s="37"/>
-      <c r="I76" s="59" t="str">
+      <c r="I76" s="57" t="str">
         <f>IF(B76="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J76" s="59" t="str">
+      <c r="J76" s="57" t="str">
         <f>IF(B76="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K76" s="60" t="str">
+      <c r="K76" s="58" t="str">
         <f>IFERROR(VLOOKUP(B76,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5645,7 +5607,7 @@
         <f>IFERROR(VLOOKUP(B77,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D77" s="58" t="str">
+      <c r="D77" s="56" t="str">
         <f>IFERROR(VLOOKUP(B77,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5653,15 +5615,15 @@
       <c r="F77" s="36"/>
       <c r="G77" s="33"/>
       <c r="H77" s="37"/>
-      <c r="I77" s="59" t="str">
+      <c r="I77" s="57" t="str">
         <f>IF(B77="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J77" s="59" t="str">
+      <c r="J77" s="57" t="str">
         <f>IF(B77="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K77" s="60" t="str">
+      <c r="K77" s="58" t="str">
         <f>IFERROR(VLOOKUP(B77,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5673,7 +5635,7 @@
         <f>IFERROR(VLOOKUP(B78,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D78" s="58" t="str">
+      <c r="D78" s="56" t="str">
         <f>IFERROR(VLOOKUP(B78,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5681,15 +5643,15 @@
       <c r="F78" s="36"/>
       <c r="G78" s="33"/>
       <c r="H78" s="37"/>
-      <c r="I78" s="59" t="str">
+      <c r="I78" s="57" t="str">
         <f>IF(B78="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J78" s="59" t="str">
+      <c r="J78" s="57" t="str">
         <f>IF(B78="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K78" s="60" t="str">
+      <c r="K78" s="58" t="str">
         <f>IFERROR(VLOOKUP(B78,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5701,7 +5663,7 @@
         <f>IFERROR(VLOOKUP(B79,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D79" s="58" t="str">
+      <c r="D79" s="56" t="str">
         <f>IFERROR(VLOOKUP(B79,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5709,15 +5671,15 @@
       <c r="F79" s="36"/>
       <c r="G79" s="33"/>
       <c r="H79" s="37"/>
-      <c r="I79" s="59" t="str">
+      <c r="I79" s="57" t="str">
         <f>IF(B79="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J79" s="59" t="str">
+      <c r="J79" s="57" t="str">
         <f>IF(B79="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K79" s="60" t="str">
+      <c r="K79" s="58" t="str">
         <f>IFERROR(VLOOKUP(B79,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5729,7 +5691,7 @@
         <f>IFERROR(VLOOKUP(B80,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D80" s="58" t="str">
+      <c r="D80" s="56" t="str">
         <f>IFERROR(VLOOKUP(B80,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5737,15 +5699,15 @@
       <c r="F80" s="36"/>
       <c r="G80" s="33"/>
       <c r="H80" s="37"/>
-      <c r="I80" s="59" t="str">
+      <c r="I80" s="57" t="str">
         <f>IF(B80="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J80" s="59" t="str">
+      <c r="J80" s="57" t="str">
         <f>IF(B80="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K80" s="60" t="str">
+      <c r="K80" s="58" t="str">
         <f>IFERROR(VLOOKUP(B80,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5757,7 +5719,7 @@
         <f>IFERROR(VLOOKUP(B81,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D81" s="58" t="str">
+      <c r="D81" s="56" t="str">
         <f>IFERROR(VLOOKUP(B81,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5765,15 +5727,15 @@
       <c r="F81" s="36"/>
       <c r="G81" s="33"/>
       <c r="H81" s="37"/>
-      <c r="I81" s="59" t="str">
+      <c r="I81" s="57" t="str">
         <f>IF(B81="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J81" s="59" t="str">
+      <c r="J81" s="57" t="str">
         <f>IF(B81="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K81" s="60" t="str">
+      <c r="K81" s="58" t="str">
         <f>IFERROR(VLOOKUP(B81,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5785,7 +5747,7 @@
         <f>IFERROR(VLOOKUP(B82,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D82" s="58" t="str">
+      <c r="D82" s="56" t="str">
         <f>IFERROR(VLOOKUP(B82,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5793,15 +5755,15 @@
       <c r="F82" s="36"/>
       <c r="G82" s="33"/>
       <c r="H82" s="37"/>
-      <c r="I82" s="59" t="str">
+      <c r="I82" s="57" t="str">
         <f>IF(B82="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J82" s="59" t="str">
+      <c r="J82" s="57" t="str">
         <f>IF(B82="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K82" s="60" t="str">
+      <c r="K82" s="58" t="str">
         <f>IFERROR(VLOOKUP(B82,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5813,7 +5775,7 @@
         <f>IFERROR(VLOOKUP(B83,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D83" s="58" t="str">
+      <c r="D83" s="56" t="str">
         <f>IFERROR(VLOOKUP(B83,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5821,15 +5783,15 @@
       <c r="F83" s="36"/>
       <c r="G83" s="33"/>
       <c r="H83" s="37"/>
-      <c r="I83" s="59" t="str">
+      <c r="I83" s="57" t="str">
         <f>IF(B83="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J83" s="59" t="str">
+      <c r="J83" s="57" t="str">
         <f>IF(B83="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K83" s="60" t="str">
+      <c r="K83" s="58" t="str">
         <f>IFERROR(VLOOKUP(B83,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5841,7 +5803,7 @@
         <f>IFERROR(VLOOKUP(B84,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D84" s="58" t="str">
+      <c r="D84" s="56" t="str">
         <f>IFERROR(VLOOKUP(B84,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5849,15 +5811,15 @@
       <c r="F84" s="36"/>
       <c r="G84" s="33"/>
       <c r="H84" s="37"/>
-      <c r="I84" s="59" t="str">
+      <c r="I84" s="57" t="str">
         <f>IF(B84="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J84" s="59" t="str">
+      <c r="J84" s="57" t="str">
         <f>IF(B84="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K84" s="60" t="str">
+      <c r="K84" s="58" t="str">
         <f>IFERROR(VLOOKUP(B84,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5869,7 +5831,7 @@
         <f>IFERROR(VLOOKUP(B85,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D85" s="58" t="str">
+      <c r="D85" s="56" t="str">
         <f>IFERROR(VLOOKUP(B85,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5877,15 +5839,15 @@
       <c r="F85" s="36"/>
       <c r="G85" s="33"/>
       <c r="H85" s="37"/>
-      <c r="I85" s="59" t="str">
+      <c r="I85" s="57" t="str">
         <f>IF(B85="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J85" s="59" t="str">
+      <c r="J85" s="57" t="str">
         <f>IF(B85="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K85" s="60" t="str">
+      <c r="K85" s="58" t="str">
         <f>IFERROR(VLOOKUP(B85,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5897,7 +5859,7 @@
         <f>IFERROR(VLOOKUP(B86,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D86" s="58" t="str">
+      <c r="D86" s="56" t="str">
         <f>IFERROR(VLOOKUP(B86,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5905,15 +5867,15 @@
       <c r="F86" s="36"/>
       <c r="G86" s="33"/>
       <c r="H86" s="37"/>
-      <c r="I86" s="59" t="str">
+      <c r="I86" s="57" t="str">
         <f>IF(B86="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J86" s="59" t="str">
+      <c r="J86" s="57" t="str">
         <f>IF(B86="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K86" s="60" t="str">
+      <c r="K86" s="58" t="str">
         <f>IFERROR(VLOOKUP(B86,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5925,7 +5887,7 @@
         <f>IFERROR(VLOOKUP(B87,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D87" s="58" t="str">
+      <c r="D87" s="56" t="str">
         <f>IFERROR(VLOOKUP(B87,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5933,15 +5895,15 @@
       <c r="F87" s="36"/>
       <c r="G87" s="33"/>
       <c r="H87" s="37"/>
-      <c r="I87" s="59" t="str">
+      <c r="I87" s="57" t="str">
         <f>IF(B87="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J87" s="59" t="str">
+      <c r="J87" s="57" t="str">
         <f>IF(B87="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K87" s="60" t="str">
+      <c r="K87" s="58" t="str">
         <f>IFERROR(VLOOKUP(B87,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5953,7 +5915,7 @@
         <f>IFERROR(VLOOKUP(B88,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D88" s="58" t="str">
+      <c r="D88" s="56" t="str">
         <f>IFERROR(VLOOKUP(B88,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5961,15 +5923,15 @@
       <c r="F88" s="36"/>
       <c r="G88" s="33"/>
       <c r="H88" s="37"/>
-      <c r="I88" s="59" t="str">
+      <c r="I88" s="57" t="str">
         <f>IF(B88="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J88" s="59" t="str">
+      <c r="J88" s="57" t="str">
         <f>IF(B88="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K88" s="60" t="str">
+      <c r="K88" s="58" t="str">
         <f>IFERROR(VLOOKUP(B88,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -5981,7 +5943,7 @@
         <f>IFERROR(VLOOKUP(B89,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D89" s="58" t="str">
+      <c r="D89" s="56" t="str">
         <f>IFERROR(VLOOKUP(B89,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -5989,15 +5951,15 @@
       <c r="F89" s="36"/>
       <c r="G89" s="33"/>
       <c r="H89" s="37"/>
-      <c r="I89" s="59" t="str">
+      <c r="I89" s="57" t="str">
         <f>IF(B89="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J89" s="59" t="str">
+      <c r="J89" s="57" t="str">
         <f>IF(B89="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K89" s="60" t="str">
+      <c r="K89" s="58" t="str">
         <f>IFERROR(VLOOKUP(B89,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -6009,7 +5971,7 @@
         <f>IFERROR(VLOOKUP(B90,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D90" s="58" t="str">
+      <c r="D90" s="56" t="str">
         <f>IFERROR(VLOOKUP(B90,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -6017,15 +5979,15 @@
       <c r="F90" s="36"/>
       <c r="G90" s="33"/>
       <c r="H90" s="37"/>
-      <c r="I90" s="59" t="str">
+      <c r="I90" s="57" t="str">
         <f>IF(B90="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J90" s="59" t="str">
+      <c r="J90" s="57" t="str">
         <f>IF(B90="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K90" s="60" t="str">
+      <c r="K90" s="58" t="str">
         <f>IFERROR(VLOOKUP(B90,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -6037,7 +5999,7 @@
         <f>IFERROR(VLOOKUP(B91,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D91" s="58" t="str">
+      <c r="D91" s="56" t="str">
         <f>IFERROR(VLOOKUP(B91,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -6045,15 +6007,15 @@
       <c r="F91" s="36"/>
       <c r="G91" s="33"/>
       <c r="H91" s="37"/>
-      <c r="I91" s="59" t="str">
+      <c r="I91" s="57" t="str">
         <f>IF(B91="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J91" s="59" t="str">
+      <c r="J91" s="57" t="str">
         <f>IF(B91="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K91" s="60" t="str">
+      <c r="K91" s="58" t="str">
         <f>IFERROR(VLOOKUP(B91,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -6065,7 +6027,7 @@
         <f>IFERROR(VLOOKUP(B92,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D92" s="58" t="str">
+      <c r="D92" s="56" t="str">
         <f>IFERROR(VLOOKUP(B92,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -6073,15 +6035,15 @@
       <c r="F92" s="36"/>
       <c r="G92" s="33"/>
       <c r="H92" s="37"/>
-      <c r="I92" s="59" t="str">
+      <c r="I92" s="57" t="str">
         <f>IF(B92="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J92" s="59" t="str">
+      <c r="J92" s="57" t="str">
         <f>IF(B92="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K92" s="60" t="str">
+      <c r="K92" s="58" t="str">
         <f>IFERROR(VLOOKUP(B92,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -6093,7 +6055,7 @@
         <f>IFERROR(VLOOKUP(B93,Names!$B$1:$E$262,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="D93" s="58" t="str">
+      <c r="D93" s="56" t="str">
         <f>IFERROR(VLOOKUP(B93,Names!$B$1:$E$262,4,FALSE),"")</f>
         <v/>
       </c>
@@ -6101,15 +6063,15 @@
       <c r="F93" s="36"/>
       <c r="G93" s="33"/>
       <c r="H93" s="37"/>
-      <c r="I93" s="59" t="str">
+      <c r="I93" s="57" t="str">
         <f>IF(B93="","",Names!$G$21)</f>
         <v/>
       </c>
-      <c r="J93" s="59" t="str">
+      <c r="J93" s="57" t="str">
         <f>IF(B93="","",Names!$H$21)</f>
         <v/>
       </c>
-      <c r="K93" s="60" t="str">
+      <c r="K93" s="58" t="str">
         <f>IFERROR(VLOOKUP(B93,Names!$B$1:$E$262,3,FALSE),"")</f>
         <v/>
       </c>
@@ -7232,17 +7194,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{55BFFC22-05E2-40B1-AB09-90A4B23CFDFD}">
+          <x14:formula1>
+            <xm:f>'Work Orders'!$B$2:$B$247</xm:f>
+          </x14:formula1>
+          <xm:sqref>F4:F159</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{57A703F9-7B94-4635-916E-38ABBFB89177}">
           <x14:formula1>
             <xm:f>Names!$B$2:$B$262</xm:f>
           </x14:formula1>
           <xm:sqref>B4:B136</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{55BFFC22-05E2-40B1-AB09-90A4B23CFDFD}">
-          <x14:formula1>
-            <xm:f>'Work Orders'!$B$2:$B$247</xm:f>
-          </x14:formula1>
-          <xm:sqref>F4:F159</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -7361,7 +7323,7 @@
         <f>'Vendor Entry Sheet'!E4</f>
         <v>0</v>
       </c>
-      <c r="H2" s="68"/>
+      <c r="H2" s="65"/>
       <c r="I2">
         <f>'Vendor Entry Sheet'!G4</f>
         <v>0</v>
@@ -21226,8 +21188,8 @@
   </sheetPr>
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21282,14 +21244,14 @@
       </c>
       <c r="B2" s="54"/>
       <c r="C2" s="55"/>
-      <c r="D2" s="54" t="s">
+      <c r="D2" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="61"/>
-      <c r="G2" s="62" t="s">
+      <c r="E2" s="59"/>
+      <c r="G2" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="66">
+      <c r="H2" s="63">
         <v>3014806</v>
       </c>
       <c r="J2" t="s">
@@ -21307,15 +21269,15 @@
         <v>573</v>
       </c>
       <c r="B3" s="54"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="54" t="s">
+      <c r="C3"/>
+      <c r="D3" t="s">
         <v>574</v>
       </c>
-      <c r="E3" s="61"/>
-      <c r="G3" s="67" t="s">
+      <c r="E3" s="59"/>
+      <c r="G3" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="66">
+      <c r="H3" s="63">
         <v>3001580</v>
       </c>
       <c r="J3" t="s">
@@ -21333,16 +21295,19 @@
         <v>573</v>
       </c>
       <c r="B4" s="54"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="54" t="s">
+      <c r="C4"/>
+      <c r="D4" t="s">
         <v>574</v>
       </c>
-      <c r="E4" s="61"/>
-      <c r="G4" s="67" t="s">
+      <c r="E4" s="59"/>
+      <c r="G4" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="67">
+      <c r="H4" s="64">
         <v>3001667</v>
+      </c>
+      <c r="J4" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -21350,117 +21315,129 @@
         <v>573</v>
       </c>
       <c r="B5" s="54"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="54" t="s">
+      <c r="C5"/>
+      <c r="D5" t="s">
         <v>574</v>
       </c>
-      <c r="E5" s="61"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
+      <c r="E5" s="59"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="J5" t="s">
+        <v>595</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
         <v>573</v>
       </c>
       <c r="B6" s="54"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="54" t="s">
+      <c r="C6"/>
+      <c r="D6" t="s">
         <v>574</v>
       </c>
-      <c r="E6" s="61"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
+      <c r="E6" s="59"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="J6" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="54" t="s">
         <v>573</v>
       </c>
       <c r="B7" s="54"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="54" t="s">
+      <c r="C7"/>
+      <c r="D7" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="61"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
+      <c r="E7" s="59"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="J7" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="54" t="s">
         <v>573</v>
       </c>
       <c r="B8" s="54"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="54" t="s">
+      <c r="C8"/>
+      <c r="D8" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="61"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
+      <c r="E8" s="59"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="J8" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="54" t="s">
         <v>573</v>
       </c>
       <c r="B9" s="54"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="54" t="s">
+      <c r="C9"/>
+      <c r="D9" t="s">
         <v>574</v>
       </c>
-      <c r="E9" s="61"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
+      <c r="E9" s="59"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="54" t="s">
         <v>573</v>
       </c>
       <c r="B10" s="54"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="54" t="s">
+      <c r="C10"/>
+      <c r="D10" t="s">
         <v>574</v>
       </c>
-      <c r="E10" s="61"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
+      <c r="E10" s="59"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="64"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="54" t="s">
         <v>573</v>
       </c>
       <c r="B11" s="54"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="54" t="s">
+      <c r="C11"/>
+      <c r="D11" t="s">
         <v>574</v>
       </c>
-      <c r="E11" s="61"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
+      <c r="E11" s="59"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="64"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="54" t="s">
         <v>573</v>
       </c>
       <c r="B12" s="54"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="54" t="s">
+      <c r="C12"/>
+      <c r="D12" t="s">
         <v>574</v>
       </c>
-      <c r="E12" s="61"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67"/>
+      <c r="E12" s="59"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="62" t="s">
+      <c r="A13" s="60" t="s">
         <v>573</v>
       </c>
-      <c r="B13" s="62"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="62" t="s">
+      <c r="B13" s="60"/>
+      <c r="C13"/>
+      <c r="D13" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="61"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
+      <c r="E13" s="59"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="54" t="s">
@@ -21469,15 +21446,15 @@
       <c r="B14" t="s">
         <v>578</v>
       </c>
-      <c r="C14" s="54">
+      <c r="C14">
         <v>90140920</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="D14" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="61"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
+      <c r="E14" s="59"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="64"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="54" t="s">
@@ -21486,13 +21463,13 @@
       <c r="B15" t="s">
         <v>579</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54" t="s">
+      <c r="C15"/>
+      <c r="D15" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="61"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67"/>
+      <c r="E15" s="59"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="54" t="s">
@@ -21501,15 +21478,15 @@
       <c r="B16" t="s">
         <v>580</v>
       </c>
-      <c r="C16" s="54">
+      <c r="C16">
         <v>90302509</v>
       </c>
-      <c r="D16" s="54" t="s">
+      <c r="D16" t="s">
         <v>575</v>
       </c>
-      <c r="E16" s="61"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
+      <c r="E16" s="59"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="64"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="54" t="s">
@@ -21518,15 +21495,15 @@
       <c r="B17" t="s">
         <v>581</v>
       </c>
-      <c r="C17" s="54">
+      <c r="C17">
         <v>90300849</v>
       </c>
-      <c r="D17" s="54" t="s">
+      <c r="D17" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="61"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
+      <c r="E17" s="59"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="64"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="54" t="s">
@@ -21535,15 +21512,15 @@
       <c r="B18" t="s">
         <v>582</v>
       </c>
-      <c r="C18" s="54">
+      <c r="C18">
         <v>90302510</v>
       </c>
-      <c r="D18" s="54" t="s">
+      <c r="D18" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="61"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="67"/>
+      <c r="E18" s="59"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="64"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="54" t="s">
@@ -21552,13 +21529,13 @@
       <c r="B19" t="s">
         <v>583</v>
       </c>
-      <c r="C19" s="54">
+      <c r="C19">
         <v>90302511</v>
       </c>
-      <c r="D19" s="54" t="s">
+      <c r="D19" t="s">
         <v>576</v>
       </c>
-      <c r="E19" s="61"/>
+      <c r="E19" s="59"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="54" t="s">
@@ -21567,13 +21544,13 @@
       <c r="B20" t="s">
         <v>584</v>
       </c>
-      <c r="C20" s="54">
+      <c r="C20">
         <v>90300016</v>
       </c>
-      <c r="D20" s="54" t="s">
+      <c r="D20" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="61"/>
+      <c r="E20" s="59"/>
       <c r="G20"/>
       <c r="H20"/>
     </row>
@@ -21584,13 +21561,13 @@
       <c r="B21" t="s">
         <v>585</v>
       </c>
-      <c r="C21" s="54">
+      <c r="C21">
         <v>90301850</v>
       </c>
-      <c r="D21" s="54" t="s">
+      <c r="D21" t="s">
         <v>577</v>
       </c>
-      <c r="E21" s="61"/>
+      <c r="E21" s="59"/>
       <c r="G21"/>
       <c r="H21"/>
     </row>
@@ -21601,13 +21578,13 @@
       <c r="B22" t="s">
         <v>586</v>
       </c>
-      <c r="C22" s="54">
+      <c r="C22">
         <v>90302512</v>
       </c>
-      <c r="D22" s="54" t="s">
+      <c r="D22" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="61"/>
+      <c r="E22" s="59"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="54" t="s">
@@ -21616,13 +21593,13 @@
       <c r="B23" t="s">
         <v>587</v>
       </c>
-      <c r="C23" s="54">
+      <c r="C23">
         <v>90137237</v>
       </c>
-      <c r="D23" s="54" t="s">
+      <c r="D23" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="61"/>
+      <c r="E23" s="59"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="54" t="s">
@@ -21631,13 +21608,13 @@
       <c r="B24" t="s">
         <v>588</v>
       </c>
-      <c r="C24" s="74">
+      <c r="C24">
         <v>90300199</v>
       </c>
-      <c r="D24" s="54" t="s">
+      <c r="D24" t="s">
         <v>575</v>
       </c>
-      <c r="E24" s="61"/>
+      <c r="E24" s="59"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="54" t="s">
@@ -21646,13 +21623,13 @@
       <c r="B25" t="s">
         <v>589</v>
       </c>
-      <c r="C25" s="54">
+      <c r="C25">
         <v>90300019</v>
       </c>
-      <c r="D25" s="54" t="s">
+      <c r="D25" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="61"/>
+      <c r="E25" s="59"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="54" t="s">
@@ -21661,13 +21638,13 @@
       <c r="B26" t="s">
         <v>590</v>
       </c>
-      <c r="C26" s="54">
+      <c r="C26">
         <v>90301314</v>
       </c>
-      <c r="D26" s="54" t="s">
+      <c r="D26" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="61"/>
+      <c r="E26" s="59"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="54" t="s">
@@ -21676,13 +21653,13 @@
       <c r="B27" t="s">
         <v>591</v>
       </c>
-      <c r="C27" s="54">
+      <c r="C27">
         <v>90302329</v>
       </c>
-      <c r="D27" s="54" t="s">
+      <c r="D27" t="s">
         <v>576</v>
       </c>
-      <c r="E27" s="61"/>
+      <c r="E27" s="59"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="54" t="s">
@@ -21691,13 +21668,13 @@
       <c r="B28" t="s">
         <v>592</v>
       </c>
-      <c r="C28" s="74">
+      <c r="C28">
         <v>90300213</v>
       </c>
-      <c r="D28" s="54" t="s">
+      <c r="D28" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="61"/>
+      <c r="E28" s="59"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="54" t="s">
@@ -21706,28 +21683,28 @@
       <c r="B29" t="s">
         <v>593</v>
       </c>
-      <c r="C29" s="74">
+      <c r="C29">
         <v>90301259</v>
       </c>
-      <c r="D29" s="54" t="s">
+      <c r="D29" t="s">
         <v>577</v>
       </c>
-      <c r="E29" s="61"/>
+      <c r="E29" s="59"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="62" t="s">
+      <c r="A30" s="60" t="s">
         <v>52</v>
       </c>
       <c r="B30" t="s">
         <v>594</v>
       </c>
-      <c r="C30" s="75">
+      <c r="C30">
         <v>90300214</v>
       </c>
-      <c r="D30" s="62" t="s">
+      <c r="D30" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="61"/>
+      <c r="E30" s="59"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="54" t="s">
@@ -21736,13 +21713,13 @@
       <c r="B31" t="s">
         <v>596</v>
       </c>
-      <c r="C31" s="76">
+      <c r="C31">
         <v>90300712</v>
       </c>
-      <c r="D31" s="54" t="s">
+      <c r="D31" t="s">
         <v>49</v>
       </c>
-      <c r="E31" s="61"/>
+      <c r="E31" s="59"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="54" t="s">
@@ -21751,13 +21728,13 @@
       <c r="B32" t="s">
         <v>597</v>
       </c>
-      <c r="C32" s="54">
+      <c r="C32">
         <v>90302495</v>
       </c>
-      <c r="D32" s="54" t="s">
+      <c r="D32" t="s">
         <v>606</v>
       </c>
-      <c r="E32" s="61" t="str">
+      <c r="E32" s="59" t="str">
         <f t="shared" ref="E32:E33" si="0">IFERROR(VLOOKUP(D32,$G$2:$H$18,2,FALSE),"")</f>
         <v/>
       </c>
@@ -21769,13 +21746,13 @@
       <c r="B33" t="s">
         <v>598</v>
       </c>
-      <c r="C33" s="54">
+      <c r="C33">
         <v>90302496</v>
       </c>
-      <c r="D33" s="54" t="s">
+      <c r="D33" t="s">
         <v>606</v>
       </c>
-      <c r="E33" s="61" t="str">
+      <c r="E33" s="59" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -21787,14 +21764,14 @@
       <c r="B34" t="s">
         <v>599</v>
       </c>
-      <c r="C34" s="54">
+      <c r="C34">
         <v>90300003</v>
       </c>
-      <c r="D34" s="54" t="s">
+      <c r="D34" t="s">
         <v>607</v>
       </c>
-      <c r="E34" s="61" t="str">
-        <f t="shared" ref="E34:E65" si="1">IFERROR(VLOOKUP(D34,$G$2:$H$18,2,FALSE),"")</f>
+      <c r="E34" s="59" t="str">
+        <f t="shared" ref="E34:E54" si="1">IFERROR(VLOOKUP(D34,$G$2:$H$18,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -21805,11 +21782,11 @@
       <c r="B35" t="s">
         <v>600</v>
       </c>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54" t="s">
+      <c r="C35"/>
+      <c r="D35" t="s">
         <v>607</v>
       </c>
-      <c r="E35" s="61" t="str">
+      <c r="E35" s="59" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -21821,13 +21798,13 @@
       <c r="B36" t="s">
         <v>601</v>
       </c>
-      <c r="C36" s="76">
+      <c r="C36">
         <v>90300039</v>
       </c>
-      <c r="D36" s="54" t="s">
+      <c r="D36" t="s">
         <v>49</v>
       </c>
-      <c r="E36" s="61"/>
+      <c r="E36" s="59"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="54" t="s">
@@ -21836,13 +21813,13 @@
       <c r="B37" t="s">
         <v>602</v>
       </c>
-      <c r="C37" s="54">
+      <c r="C37">
         <v>90144128</v>
       </c>
-      <c r="D37" s="54" t="s">
+      <c r="D37" t="s">
         <v>606</v>
       </c>
-      <c r="E37" s="61" t="str">
+      <c r="E37" s="59" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -21854,13 +21831,13 @@
       <c r="B38" t="s">
         <v>603</v>
       </c>
-      <c r="C38" s="54">
+      <c r="C38">
         <v>90302497</v>
       </c>
-      <c r="D38" s="54" t="s">
+      <c r="D38" t="s">
         <v>606</v>
       </c>
-      <c r="E38" s="61" t="str">
+      <c r="E38" s="59" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -21872,31 +21849,31 @@
       <c r="B39" t="s">
         <v>604</v>
       </c>
-      <c r="C39" s="54">
+      <c r="C39">
         <v>90301392</v>
       </c>
-      <c r="D39" s="54" t="s">
+      <c r="D39" t="s">
         <v>607</v>
       </c>
-      <c r="E39" s="61" t="str">
+      <c r="E39" s="59" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="62" t="s">
+      <c r="A40" s="60" t="s">
         <v>595</v>
       </c>
       <c r="B40" t="s">
         <v>605</v>
       </c>
-      <c r="C40" s="62">
+      <c r="C40">
         <v>90302498</v>
       </c>
-      <c r="D40" s="62" t="s">
+      <c r="D40" t="s">
         <v>607</v>
       </c>
-      <c r="E40" s="61" t="str">
+      <c r="E40" s="59" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -21905,111 +21882,111 @@
       <c r="A41" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B41" s="64"/>
-      <c r="C41" s="65"/>
-      <c r="D41" s="54" t="s">
+      <c r="B41" s="61"/>
+      <c r="C41"/>
+      <c r="D41" t="s">
         <v>49</v>
       </c>
-      <c r="E41" s="61"/>
+      <c r="E41" s="59"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B42" s="64"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="54" t="s">
+      <c r="B42" s="61"/>
+      <c r="C42"/>
+      <c r="D42" t="s">
         <v>606</v>
       </c>
-      <c r="E42" s="61"/>
+      <c r="E42" s="59"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B43" s="64"/>
-      <c r="C43" s="65"/>
-      <c r="D43" s="54" t="s">
+      <c r="B43" s="61"/>
+      <c r="C43"/>
+      <c r="D43" t="s">
         <v>606</v>
       </c>
-      <c r="E43" s="61"/>
+      <c r="E43" s="59"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B44" s="64"/>
-      <c r="C44" s="65"/>
-      <c r="D44" s="54" t="s">
+      <c r="B44" s="61"/>
+      <c r="C44"/>
+      <c r="D44" t="s">
         <v>607</v>
       </c>
-      <c r="E44" s="61"/>
+      <c r="E44" s="59"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="64"/>
-      <c r="C45" s="65"/>
-      <c r="D45" s="54" t="s">
+      <c r="B45" s="61"/>
+      <c r="C45"/>
+      <c r="D45" t="s">
         <v>606</v>
       </c>
-      <c r="E45" s="61"/>
+      <c r="E45" s="59"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="64"/>
-      <c r="C46" s="65"/>
-      <c r="D46" s="54" t="s">
+      <c r="B46" s="61"/>
+      <c r="C46"/>
+      <c r="D46" t="s">
         <v>606</v>
       </c>
-      <c r="E46" s="61"/>
+      <c r="E46" s="59"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="64"/>
-      <c r="C47" s="65"/>
-      <c r="D47" s="54" t="s">
+      <c r="B47" s="61"/>
+      <c r="C47"/>
+      <c r="D47" t="s">
         <v>607</v>
       </c>
-      <c r="E47" s="61"/>
+      <c r="E47" s="59"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="64"/>
-      <c r="C48" s="65"/>
-      <c r="D48" s="54" t="s">
+      <c r="B48" s="61"/>
+      <c r="C48"/>
+      <c r="D48" t="s">
         <v>49</v>
       </c>
-      <c r="E48" s="61"/>
+      <c r="E48" s="59"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="64"/>
-      <c r="C49" s="65"/>
-      <c r="D49" s="54" t="s">
+      <c r="B49" s="61"/>
+      <c r="C49"/>
+      <c r="D49" t="s">
         <v>606</v>
       </c>
-      <c r="E49" s="61"/>
+      <c r="E49" s="59"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B50" s="64"/>
-      <c r="C50" s="65"/>
-      <c r="D50" s="54" t="s">
+      <c r="B50" s="61"/>
+      <c r="C50"/>
+      <c r="D50" t="s">
         <v>606</v>
       </c>
-      <c r="E50" s="61" t="str">
+      <c r="E50" s="59" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -22018,12 +21995,12 @@
       <c r="A51" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B51" s="64"/>
-      <c r="C51" s="65"/>
-      <c r="D51" s="54" t="s">
+      <c r="B51" s="61"/>
+      <c r="C51"/>
+      <c r="D51" t="s">
         <v>607</v>
       </c>
-      <c r="E51" s="61" t="str">
+      <c r="E51" s="59" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -22032,12 +22009,12 @@
       <c r="A52" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="64"/>
-      <c r="C52" s="65"/>
-      <c r="D52" s="54" t="s">
+      <c r="B52" s="61"/>
+      <c r="C52"/>
+      <c r="D52" t="s">
         <v>606</v>
       </c>
-      <c r="E52" s="61" t="str">
+      <c r="E52" s="59" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -22046,26 +22023,26 @@
       <c r="A53" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B53" s="64"/>
-      <c r="C53" s="65"/>
-      <c r="D53" s="54" t="s">
+      <c r="B53" s="61"/>
+      <c r="C53"/>
+      <c r="D53" t="s">
         <v>606</v>
       </c>
-      <c r="E53" s="61" t="str">
+      <c r="E53" s="59" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="62" t="s">
+      <c r="A54" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="B54" s="64"/>
-      <c r="C54" s="65"/>
-      <c r="D54" s="62" t="s">
+      <c r="B54" s="61"/>
+      <c r="C54"/>
+      <c r="D54" t="s">
         <v>607</v>
       </c>
-      <c r="E54" s="61" t="str">
+      <c r="E54" s="59" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -22074,12 +22051,12 @@
       <c r="A55" s="54" t="s">
         <v>570</v>
       </c>
-      <c r="B55" s="64"/>
-      <c r="C55" s="65"/>
-      <c r="D55" s="54" t="s">
+      <c r="B55" s="61"/>
+      <c r="C55"/>
+      <c r="D55" t="s">
         <v>49</v>
       </c>
-      <c r="E55" s="61"/>
+      <c r="E55" s="59"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="54" t="s">
@@ -22088,13 +22065,13 @@
       <c r="B56" t="s">
         <v>608</v>
       </c>
-      <c r="C56" s="54">
+      <c r="C56">
         <v>90300462</v>
       </c>
-      <c r="D56" s="54" t="s">
+      <c r="D56" t="s">
         <v>606</v>
       </c>
-      <c r="E56" s="61"/>
+      <c r="E56" s="59"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="54" t="s">
@@ -22103,13 +22080,13 @@
       <c r="B57" t="s">
         <v>609</v>
       </c>
-      <c r="C57" s="54">
+      <c r="C57">
         <v>90302117</v>
       </c>
-      <c r="D57" s="54" t="s">
+      <c r="D57" t="s">
         <v>607</v>
       </c>
-      <c r="E57" s="61"/>
+      <c r="E57" s="59"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="54" t="s">
@@ -22118,11 +22095,11 @@
       <c r="B58" t="s">
         <v>610</v>
       </c>
-      <c r="C58" s="54"/>
-      <c r="D58" s="54" t="s">
+      <c r="C58"/>
+      <c r="D58" t="s">
         <v>48</v>
       </c>
-      <c r="E58" s="61"/>
+      <c r="E58" s="59"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="54" t="s">
@@ -22131,13 +22108,13 @@
       <c r="B59" t="s">
         <v>611</v>
       </c>
-      <c r="C59" s="54">
+      <c r="C59">
         <v>90300586</v>
       </c>
-      <c r="D59" s="54" t="s">
+      <c r="D59" t="s">
         <v>606</v>
       </c>
-      <c r="E59" s="61"/>
+      <c r="E59" s="59"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="54" t="s">
@@ -22146,13 +22123,13 @@
       <c r="B60" t="s">
         <v>612</v>
       </c>
-      <c r="C60" s="54">
+      <c r="C60">
         <v>90302487</v>
       </c>
-      <c r="D60" s="54" t="s">
+      <c r="D60" t="s">
         <v>607</v>
       </c>
-      <c r="E60" s="61"/>
+      <c r="E60" s="59"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="54" t="s">
@@ -22161,13 +22138,13 @@
       <c r="B61" t="s">
         <v>613</v>
       </c>
-      <c r="C61" s="54">
+      <c r="C61">
         <v>90302465</v>
       </c>
-      <c r="D61" s="54" t="s">
+      <c r="D61" t="s">
         <v>48</v>
       </c>
-      <c r="E61" s="61"/>
+      <c r="E61" s="59"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="54" t="s">
@@ -22176,13 +22153,13 @@
       <c r="B62" t="s">
         <v>614</v>
       </c>
-      <c r="C62" s="54">
+      <c r="C62">
         <v>90117360</v>
       </c>
-      <c r="D62" s="54" t="s">
+      <c r="D62" t="s">
         <v>49</v>
       </c>
-      <c r="E62" s="61"/>
+      <c r="E62" s="59"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="54" t="s">
@@ -22191,13 +22168,13 @@
       <c r="B63" t="s">
         <v>615</v>
       </c>
-      <c r="C63" s="54">
+      <c r="C63">
         <v>90302118</v>
       </c>
-      <c r="D63" s="54" t="s">
+      <c r="D63" t="s">
         <v>606</v>
       </c>
-      <c r="E63" s="61"/>
+      <c r="E63" s="59"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="54" t="s">
@@ -22206,13 +22183,13 @@
       <c r="B64" t="s">
         <v>616</v>
       </c>
-      <c r="C64" s="76">
+      <c r="C64">
         <v>90144804</v>
       </c>
-      <c r="D64" s="54" t="s">
+      <c r="D64" t="s">
         <v>607</v>
       </c>
-      <c r="E64" s="61"/>
+      <c r="E64" s="59"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="54" t="s">
@@ -22221,13 +22198,13 @@
       <c r="B65" t="s">
         <v>617</v>
       </c>
-      <c r="C65" s="76">
+      <c r="C65">
         <v>90302398</v>
       </c>
-      <c r="D65" s="54" t="s">
+      <c r="D65" t="s">
         <v>48</v>
       </c>
-      <c r="E65" s="61"/>
+      <c r="E65" s="59"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="54" t="s">
@@ -22236,13 +22213,13 @@
       <c r="B66" t="s">
         <v>618</v>
       </c>
-      <c r="C66" s="54">
+      <c r="C66">
         <v>90302503</v>
       </c>
-      <c r="D66" s="54" t="s">
+      <c r="D66" t="s">
         <v>606</v>
       </c>
-      <c r="E66" s="61"/>
+      <c r="E66" s="59"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="54" t="s">
@@ -22251,377 +22228,377 @@
       <c r="B67" t="s">
         <v>619</v>
       </c>
-      <c r="C67" s="76">
+      <c r="C67">
         <v>90302504</v>
       </c>
-      <c r="D67" s="54" t="s">
+      <c r="D67" t="s">
         <v>607</v>
       </c>
-      <c r="E67" s="61"/>
+      <c r="E67" s="59"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="62" t="s">
+      <c r="A68" s="60" t="s">
         <v>570</v>
       </c>
       <c r="B68" t="s">
         <v>620</v>
       </c>
-      <c r="C68" s="63"/>
-      <c r="D68" s="62" t="s">
+      <c r="C68"/>
+      <c r="D68" t="s">
         <v>48</v>
       </c>
-      <c r="E68" s="65"/>
+      <c r="E68" s="62"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="62" t="s">
+      <c r="A69" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B69" t="s">
         <v>623</v>
       </c>
-      <c r="C69" s="74">
+      <c r="C69">
         <v>90290068</v>
       </c>
-      <c r="D69" s="54" t="s">
+      <c r="D69" t="s">
         <v>49</v>
       </c>
-      <c r="E69" s="65" t="str">
+      <c r="E69" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="62" t="s">
+      <c r="A70" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B70" t="s">
         <v>624</v>
       </c>
-      <c r="C70" s="74">
+      <c r="C70">
         <v>90302469</v>
       </c>
-      <c r="D70" s="54" t="s">
+      <c r="D70" t="s">
         <v>606</v>
       </c>
-      <c r="E70" s="65" t="str">
+      <c r="E70" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="62" t="s">
+      <c r="A71" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B71" t="s">
         <v>625</v>
       </c>
-      <c r="C71" s="74">
+      <c r="C71">
         <v>90302453</v>
       </c>
-      <c r="D71" s="54" t="s">
+      <c r="D71" t="s">
         <v>606</v>
       </c>
-      <c r="E71" s="65" t="str">
+      <c r="E71" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="62" t="s">
+      <c r="A72" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B72" t="s">
         <v>626</v>
       </c>
-      <c r="C72" s="76">
+      <c r="C72">
         <v>90301928</v>
       </c>
-      <c r="D72" s="54" t="s">
+      <c r="D72" t="s">
         <v>607</v>
       </c>
-      <c r="E72" s="65" t="str">
+      <c r="E72" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="62" t="s">
+      <c r="A73" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B73" t="s">
         <v>627</v>
       </c>
-      <c r="C73" s="74">
+      <c r="C73">
         <v>90302455</v>
       </c>
-      <c r="D73" s="54" t="s">
+      <c r="D73" t="s">
         <v>622</v>
       </c>
-      <c r="E73" s="65" t="str">
+      <c r="E73" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="62" t="s">
+      <c r="A74" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B74" t="s">
         <v>628</v>
       </c>
-      <c r="C74" s="76">
+      <c r="C74">
         <v>90302470</v>
       </c>
-      <c r="D74" s="54" t="s">
+      <c r="D74" t="s">
         <v>48</v>
       </c>
-      <c r="E74" s="65" t="str">
+      <c r="E74" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="62" t="s">
+      <c r="A75" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B75" t="s">
         <v>629</v>
       </c>
-      <c r="C75" s="74">
+      <c r="C75">
         <v>90302471</v>
       </c>
-      <c r="D75" s="54" t="s">
+      <c r="D75" t="s">
         <v>48</v>
       </c>
-      <c r="E75" s="65" t="str">
+      <c r="E75" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="62" t="s">
+      <c r="A76" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B76" t="s">
         <v>630</v>
       </c>
-      <c r="C76" s="74">
+      <c r="C76">
         <v>90302457</v>
       </c>
-      <c r="D76" s="54" t="s">
+      <c r="D76" t="s">
         <v>606</v>
       </c>
-      <c r="E76" s="65" t="str">
+      <c r="E76" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="62" t="s">
+      <c r="A77" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B77" t="s">
         <v>600</v>
       </c>
-      <c r="C77" s="65"/>
-      <c r="D77" s="54" t="s">
+      <c r="C77"/>
+      <c r="D77" t="s">
         <v>606</v>
       </c>
-      <c r="E77" s="65" t="str">
+      <c r="E77" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="62" t="s">
+      <c r="A78" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B78" t="s">
         <v>631</v>
       </c>
-      <c r="C78" s="74">
+      <c r="C78">
         <v>90290075</v>
       </c>
-      <c r="D78" s="54" t="s">
+      <c r="D78" t="s">
         <v>607</v>
       </c>
-      <c r="E78" s="65" t="str">
+      <c r="E78" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="62" t="s">
+      <c r="A79" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B79" t="s">
         <v>632</v>
       </c>
-      <c r="C79" s="54">
+      <c r="C79">
         <v>90302218</v>
       </c>
-      <c r="D79" s="54" t="s">
+      <c r="D79" t="s">
         <v>622</v>
       </c>
-      <c r="E79" s="65" t="str">
+      <c r="E79" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="62" t="s">
+      <c r="A80" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B80" t="s">
         <v>633</v>
       </c>
-      <c r="C80" s="77">
+      <c r="C80">
         <v>90290074</v>
       </c>
-      <c r="D80" s="62" t="s">
+      <c r="D80" t="s">
         <v>49</v>
       </c>
-      <c r="E80" s="65" t="str">
+      <c r="E80" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="62" t="s">
+      <c r="A81" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B81" t="s">
         <v>635</v>
       </c>
-      <c r="C81" s="77">
+      <c r="C81">
         <v>90301453</v>
       </c>
-      <c r="D81" s="62" t="s">
+      <c r="D81" t="s">
         <v>49</v>
       </c>
-      <c r="E81" s="65"/>
+      <c r="E81" s="62"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="62" t="s">
+      <c r="A82" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B82" t="s">
         <v>636</v>
       </c>
-      <c r="C82" s="75">
+      <c r="C82">
         <v>90300620</v>
       </c>
-      <c r="D82" s="62" t="s">
+      <c r="D82" t="s">
         <v>634</v>
       </c>
-      <c r="E82" s="65"/>
+      <c r="E82" s="62"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="62" t="s">
+      <c r="A83" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B83" t="s">
         <v>637</v>
       </c>
-      <c r="C83" s="75">
+      <c r="C83">
         <v>90290069</v>
       </c>
-      <c r="D83" s="62" t="s">
+      <c r="D83" t="s">
         <v>634</v>
       </c>
-      <c r="E83" s="65"/>
+      <c r="E83" s="62"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="62" t="s">
+      <c r="A84" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B84" t="s">
         <v>638</v>
       </c>
-      <c r="C84" s="75">
+      <c r="C84">
         <v>90290077</v>
       </c>
-      <c r="D84" s="62" t="s">
+      <c r="D84" t="s">
         <v>634</v>
       </c>
-      <c r="E84" s="65"/>
+      <c r="E84" s="62"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="62" t="s">
+      <c r="A85" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B85" t="s">
         <v>639</v>
       </c>
-      <c r="C85" s="77">
+      <c r="C85">
         <v>90301388</v>
       </c>
-      <c r="D85" s="62" t="s">
+      <c r="D85" t="s">
         <v>49</v>
       </c>
-      <c r="E85" s="65"/>
+      <c r="E85" s="62"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="62" t="s">
+      <c r="A86" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B86" t="s">
         <v>640</v>
       </c>
-      <c r="C86" s="62">
+      <c r="C86">
         <v>90302500</v>
       </c>
-      <c r="D86" s="62" t="s">
+      <c r="D86" t="s">
         <v>634</v>
       </c>
-      <c r="E86" s="65"/>
+      <c r="E86" s="62"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="62" t="s">
+      <c r="A87" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B87" t="s">
         <v>641</v>
       </c>
-      <c r="C87" s="77">
+      <c r="C87">
         <v>90302088</v>
       </c>
-      <c r="D87" s="62" t="s">
+      <c r="D87" t="s">
         <v>634</v>
       </c>
-      <c r="E87" s="65" t="str">
-        <f t="shared" ref="E66:E97" si="2">IFERROR(VLOOKUP(D87,$G$2:$H$18,2,FALSE),"")</f>
+      <c r="E87" s="62" t="str">
+        <f t="shared" ref="E87:E89" si="2">IFERROR(VLOOKUP(D87,$G$2:$H$18,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="62" t="s">
+      <c r="A88" s="60" t="s">
         <v>621</v>
       </c>
       <c r="B88" t="s">
         <v>642</v>
       </c>
-      <c r="C88" s="77">
+      <c r="C88">
         <v>90302447</v>
       </c>
-      <c r="D88" s="62" t="s">
+      <c r="D88" t="s">
         <v>634</v>
       </c>
-      <c r="E88" s="65" t="str">
+      <c r="E88" s="62" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="62" t="s">
+      <c r="A89" s="60" t="s">
         <v>643</v>
       </c>
-      <c r="B89" s="64"/>
-      <c r="C89" s="65"/>
-      <c r="D89" s="62" t="s">
+      <c r="B89" s="61"/>
+      <c r="C89"/>
+      <c r="D89" t="s">
         <v>644</v>
       </c>
-      <c r="E89" s="65" t="str">
+      <c r="E89" s="62" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -22630,209 +22607,201 @@
       <c r="A90" s="54" t="s">
         <v>645</v>
       </c>
-      <c r="B90" s="64"/>
-      <c r="C90" s="54">
+      <c r="B90" t="s">
+        <v>648</v>
+      </c>
+      <c r="C90">
         <v>90101732</v>
       </c>
-      <c r="D90" s="54" t="s">
+      <c r="D90" t="s">
         <v>49</v>
-      </c>
-      <c r="E90" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="54" t="s">
         <v>645</v>
       </c>
-      <c r="B91" s="64"/>
-      <c r="C91" s="54">
+      <c r="B91" t="s">
+        <v>649</v>
+      </c>
+      <c r="C91">
         <v>90302038</v>
       </c>
-      <c r="D91" s="54" t="s">
+      <c r="D91" t="s">
         <v>646</v>
-      </c>
-      <c r="E91" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="54" t="s">
         <v>645</v>
       </c>
-      <c r="B92" s="64"/>
-      <c r="C92" s="54">
+      <c r="B92" t="s">
+        <v>650</v>
+      </c>
+      <c r="C92">
         <v>90301852</v>
       </c>
-      <c r="D92" s="54" t="s">
+      <c r="D92" t="s">
         <v>646</v>
-      </c>
-      <c r="E92" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="54" t="s">
         <v>645</v>
       </c>
-      <c r="B93" s="64"/>
-      <c r="C93" s="54">
+      <c r="B93" t="s">
+        <v>651</v>
+      </c>
+      <c r="C93">
         <v>90128100</v>
       </c>
-      <c r="D93" s="54" t="s">
+      <c r="D93" t="s">
         <v>49</v>
-      </c>
-      <c r="E93" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="54" t="s">
         <v>645</v>
       </c>
-      <c r="B94" s="64"/>
-      <c r="C94" s="76">
+      <c r="B94" t="s">
+        <v>652</v>
+      </c>
+      <c r="C94">
         <v>90290053</v>
       </c>
-      <c r="D94" s="54" t="s">
+      <c r="D94" t="s">
         <v>646</v>
-      </c>
-      <c r="E94" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="54" t="s">
         <v>645</v>
       </c>
-      <c r="B95" s="64"/>
-      <c r="C95" s="54">
+      <c r="B95" t="s">
+        <v>653</v>
+      </c>
+      <c r="C95">
         <v>90300229</v>
       </c>
-      <c r="D95" s="54" t="s">
+      <c r="D95" t="s">
         <v>646</v>
-      </c>
-      <c r="E95" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="54" t="s">
         <v>645</v>
       </c>
-      <c r="B96" s="64"/>
-      <c r="C96" s="76">
+      <c r="B96" t="s">
+        <v>654</v>
+      </c>
+      <c r="C96">
         <v>90301651</v>
       </c>
-      <c r="D96" s="54" t="s">
+      <c r="D96" t="s">
         <v>647</v>
-      </c>
-      <c r="E96" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="54" t="s">
         <v>645</v>
       </c>
-      <c r="C97" s="76">
+      <c r="B97" t="s">
+        <v>655</v>
+      </c>
+      <c r="C97">
         <v>90302044</v>
       </c>
-      <c r="D97" s="54" t="s">
+      <c r="D97" t="s">
         <v>647</v>
-      </c>
-      <c r="E97" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="54" t="s">
         <v>645</v>
       </c>
-      <c r="C98" s="76">
+      <c r="B98" t="s">
+        <v>656</v>
+      </c>
+      <c r="C98">
         <v>90300312</v>
       </c>
-      <c r="D98" s="54" t="s">
+      <c r="D98" t="s">
         <v>647</v>
-      </c>
-      <c r="E98" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="54" t="s">
         <v>645</v>
       </c>
-      <c r="C99" s="76">
+      <c r="B99" t="s">
+        <v>657</v>
+      </c>
+      <c r="C99">
         <v>90300287</v>
       </c>
-      <c r="D99" s="54" t="s">
+      <c r="D99" t="s">
         <v>647</v>
-      </c>
-      <c r="E99" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="54" t="s">
         <v>645</v>
       </c>
-      <c r="C100" s="76">
+      <c r="B100" t="s">
+        <v>658</v>
+      </c>
+      <c r="C100">
         <v>90300546</v>
       </c>
-      <c r="D100" s="54" t="s">
+      <c r="D100" t="s">
         <v>647</v>
-      </c>
-      <c r="E100" t="s">
-        <v>658</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="54" t="s">
         <v>645</v>
       </c>
-      <c r="C101" s="76">
+      <c r="B101" t="s">
+        <v>659</v>
+      </c>
+      <c r="C101">
         <v>90300274</v>
       </c>
-      <c r="D101" s="54" t="s">
+      <c r="D101" t="s">
         <v>647</v>
-      </c>
-      <c r="E101" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="54" t="s">
         <v>645</v>
       </c>
-      <c r="C102" s="76">
+      <c r="B102" t="s">
+        <v>660</v>
+      </c>
+      <c r="C102">
         <v>90300281</v>
       </c>
-      <c r="D102" s="54" t="s">
+      <c r="D102" t="s">
         <v>647</v>
       </c>
-      <c r="E102" t="s">
-        <v>660</v>
-      </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="62" t="s">
+      <c r="A103" s="60" t="s">
         <v>645</v>
       </c>
-      <c r="B103" s="64"/>
-      <c r="C103" s="78">
+      <c r="B103" t="s">
+        <v>661</v>
+      </c>
+      <c r="C103">
         <v>90302337</v>
       </c>
-      <c r="D103" s="62" t="s">
+      <c r="D103" t="s">
         <v>647</v>
-      </c>
-      <c r="E103" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E104" s="11" t="str">
-        <f t="shared" ref="E98:E110" si="3">IFERROR(VLOOKUP(D104,$G$2:$H$18,2,FALSE),"")</f>
+        <f t="shared" ref="E104:E110" si="3">IFERROR(VLOOKUP(D104,$G$2:$H$18,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -22885,7 +22854,7 @@
   </sheetPr>
   <dimension ref="A1:F397"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
@@ -22899,22 +22868,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="66" t="s">
         <v>53</v>
       </c>
     </row>
@@ -30381,17 +30350,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a1bbf4fc-2070-4842-8cf2-c42346818ea9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d41b7399-51ed-4fce-9e89-79a41c55ed41">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004A5BF6C7F67B434096FAC9443A83D821" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1347de4a6797875f8d6b1ac5dc93737c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d41b7399-51ed-4fce-9e89-79a41c55ed41" xmlns:ns3="a1bbf4fc-2070-4842-8cf2-c42346818ea9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="67ec082bb3101a8db1bb88f037f675cb" ns2:_="" ns3:_="">
     <xsd:import namespace="d41b7399-51ed-4fce-9e89-79a41c55ed41"/>
@@ -30634,6 +30592,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a1bbf4fc-2070-4842-8cf2-c42346818ea9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d41b7399-51ed-4fce-9e89-79a41c55ed41">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71C3BF75-E265-495B-A1EF-9F0F8014FF62}">
   <ds:schemaRefs>
@@ -30643,17 +30612,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C286B8F-44DD-46A1-8664-5B3AFC40D364}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a1bbf4fc-2070-4842-8cf2-c42346818ea9"/>
-    <ds:schemaRef ds:uri="d41b7399-51ed-4fce-9e89-79a41c55ed41"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F00606B-6B80-42B0-B0DE-C79F0839CF7D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -30670,4 +30628,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C286B8F-44DD-46A1-8664-5B3AFC40D364}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a1bbf4fc-2070-4842-8cf2-c42346818ea9"/>
+    <ds:schemaRef ds:uri="d41b7399-51ed-4fce-9e89-79a41c55ed41"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update Excel template SMS
</commit_message>
<xml_diff>
--- a/public/data/Master App Timesheet.xlsx
+++ b/public/data/Master App Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgelD\timesheet-app\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03989A7-30A1-494C-BD18-814BE3503E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F91DB55-F499-47BC-8C11-D34953F2425E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendor Entry Sheet" sheetId="5" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2896" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2896" uniqueCount="661">
   <si>
     <t xml:space="preserve">Date
 </t>
@@ -1810,9 +1810,6 @@
   </si>
   <si>
     <t>Minprovise</t>
-  </si>
-  <si>
-    <t>SMS</t>
   </si>
   <si>
     <t>Kings</t>
@@ -21188,7 +21185,7 @@
   </sheetPr>
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
@@ -21240,7 +21237,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B2" s="54"/>
       <c r="C2" s="55"/>
@@ -21266,12 +21263,12 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B3" s="54"/>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E3" s="59"/>
       <c r="G3" s="64" t="s">
@@ -21292,12 +21289,12 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="54" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B4" s="54"/>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E4" s="59"/>
       <c r="G4" s="64" t="s">
@@ -21307,44 +21304,44 @@
         <v>3001667</v>
       </c>
       <c r="J4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B5" s="54"/>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E5" s="59"/>
       <c r="G5" s="64"/>
       <c r="H5" s="64"/>
       <c r="J5" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B6" s="54"/>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E6" s="59"/>
       <c r="G6" s="64"/>
       <c r="H6" s="64"/>
       <c r="J6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="54" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B7" s="54"/>
       <c r="C7"/>
@@ -21360,7 +21357,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="54" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B8" s="54"/>
       <c r="C8"/>
@@ -21371,17 +21368,17 @@
       <c r="G8" s="64"/>
       <c r="H8" s="64"/>
       <c r="J8" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="54" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B9" s="54"/>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E9" s="59"/>
       <c r="G9" s="64"/>
@@ -21389,12 +21386,12 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="54" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B10" s="54"/>
       <c r="C10"/>
       <c r="D10" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E10" s="59"/>
       <c r="G10" s="64"/>
@@ -21402,12 +21399,12 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="54" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B11" s="54"/>
       <c r="C11"/>
       <c r="D11" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E11" s="59"/>
       <c r="G11" s="64"/>
@@ -21415,12 +21412,12 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="54" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B12" s="54"/>
       <c r="C12"/>
       <c r="D12" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E12" s="59"/>
       <c r="G12" s="64"/>
@@ -21428,7 +21425,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="60" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B13" s="60"/>
       <c r="C13"/>
@@ -21444,7 +21441,7 @@
         <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C14">
         <v>90140920</v>
@@ -21461,7 +21458,7 @@
         <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
@@ -21476,13 +21473,13 @@
         <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C16">
         <v>90302509</v>
       </c>
       <c r="D16" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E16" s="59"/>
       <c r="G16" s="64"/>
@@ -21493,7 +21490,7 @@
         <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C17">
         <v>90300849</v>
@@ -21510,7 +21507,7 @@
         <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C18">
         <v>90302510</v>
@@ -21527,13 +21524,13 @@
         <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C19">
         <v>90302511</v>
       </c>
       <c r="D19" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E19" s="59"/>
     </row>
@@ -21542,7 +21539,7 @@
         <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C20">
         <v>90300016</v>
@@ -21559,13 +21556,13 @@
         <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C21">
         <v>90301850</v>
       </c>
       <c r="D21" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E21" s="59"/>
       <c r="G21"/>
@@ -21576,7 +21573,7 @@
         <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C22">
         <v>90302512</v>
@@ -21591,7 +21588,7 @@
         <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C23">
         <v>90137237</v>
@@ -21606,13 +21603,13 @@
         <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C24">
         <v>90300199</v>
       </c>
       <c r="D24" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E24" s="59"/>
     </row>
@@ -21621,7 +21618,7 @@
         <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C25">
         <v>90300019</v>
@@ -21636,7 +21633,7 @@
         <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C26">
         <v>90301314</v>
@@ -21651,13 +21648,13 @@
         <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C27">
         <v>90302329</v>
       </c>
       <c r="D27" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E27" s="59"/>
     </row>
@@ -21666,7 +21663,7 @@
         <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C28">
         <v>90300213</v>
@@ -21681,13 +21678,13 @@
         <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C29">
         <v>90301259</v>
       </c>
       <c r="D29" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E29" s="59"/>
     </row>
@@ -21696,7 +21693,7 @@
         <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C30">
         <v>90300214</v>
@@ -21708,10 +21705,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="54" t="s">
+        <v>594</v>
+      </c>
+      <c r="B31" t="s">
         <v>595</v>
-      </c>
-      <c r="B31" t="s">
-        <v>596</v>
       </c>
       <c r="C31">
         <v>90300712</v>
@@ -21723,16 +21720,16 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="54" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B32" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C32">
         <v>90302495</v>
       </c>
       <c r="D32" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E32" s="59" t="str">
         <f t="shared" ref="E32:E33" si="0">IFERROR(VLOOKUP(D32,$G$2:$H$18,2,FALSE),"")</f>
@@ -21741,16 +21738,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="54" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B33" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C33">
         <v>90302496</v>
       </c>
       <c r="D33" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E33" s="59" t="str">
         <f t="shared" si="0"/>
@@ -21759,16 +21756,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="54" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B34" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C34">
         <v>90300003</v>
       </c>
       <c r="D34" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E34" s="59" t="str">
         <f t="shared" ref="E34:E54" si="1">IFERROR(VLOOKUP(D34,$G$2:$H$18,2,FALSE),"")</f>
@@ -21777,14 +21774,14 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="54" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B35" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C35"/>
       <c r="D35" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E35" s="59" t="str">
         <f t="shared" si="1"/>
@@ -21793,10 +21790,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="54" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B36" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C36">
         <v>90300039</v>
@@ -21808,16 +21805,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="54" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B37" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C37">
         <v>90144128</v>
       </c>
       <c r="D37" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E37" s="59" t="str">
         <f t="shared" si="1"/>
@@ -21826,16 +21823,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="54" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B38" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C38">
         <v>90302497</v>
       </c>
       <c r="D38" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E38" s="59" t="str">
         <f t="shared" si="1"/>
@@ -21844,16 +21841,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="54" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B39" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C39">
         <v>90301392</v>
       </c>
       <c r="D39" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E39" s="59" t="str">
         <f t="shared" si="1"/>
@@ -21862,16 +21859,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="60" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B40" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C40">
         <v>90302498</v>
       </c>
       <c r="D40" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E40" s="59" t="str">
         <f t="shared" si="1"/>
@@ -21896,7 +21893,7 @@
       <c r="B42" s="61"/>
       <c r="C42"/>
       <c r="D42" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E42" s="59"/>
     </row>
@@ -21907,7 +21904,7 @@
       <c r="B43" s="61"/>
       <c r="C43"/>
       <c r="D43" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E43" s="59"/>
     </row>
@@ -21918,7 +21915,7 @@
       <c r="B44" s="61"/>
       <c r="C44"/>
       <c r="D44" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E44" s="59"/>
     </row>
@@ -21929,7 +21926,7 @@
       <c r="B45" s="61"/>
       <c r="C45"/>
       <c r="D45" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E45" s="59"/>
     </row>
@@ -21940,7 +21937,7 @@
       <c r="B46" s="61"/>
       <c r="C46"/>
       <c r="D46" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E46" s="59"/>
     </row>
@@ -21951,7 +21948,7 @@
       <c r="B47" s="61"/>
       <c r="C47"/>
       <c r="D47" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E47" s="59"/>
     </row>
@@ -21973,7 +21970,7 @@
       <c r="B49" s="61"/>
       <c r="C49"/>
       <c r="D49" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E49" s="59"/>
     </row>
@@ -21984,7 +21981,7 @@
       <c r="B50" s="61"/>
       <c r="C50"/>
       <c r="D50" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E50" s="59" t="str">
         <f t="shared" si="1"/>
@@ -21998,7 +21995,7 @@
       <c r="B51" s="61"/>
       <c r="C51"/>
       <c r="D51" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E51" s="59" t="str">
         <f t="shared" si="1"/>
@@ -22012,7 +22009,7 @@
       <c r="B52" s="61"/>
       <c r="C52"/>
       <c r="D52" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E52" s="59" t="str">
         <f t="shared" si="1"/>
@@ -22026,7 +22023,7 @@
       <c r="B53" s="61"/>
       <c r="C53"/>
       <c r="D53" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E53" s="59" t="str">
         <f t="shared" si="1"/>
@@ -22040,7 +22037,7 @@
       <c r="B54" s="61"/>
       <c r="C54"/>
       <c r="D54" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E54" s="59" t="str">
         <f t="shared" si="1"/>
@@ -22063,13 +22060,13 @@
         <v>570</v>
       </c>
       <c r="B56" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C56">
         <v>90300462</v>
       </c>
       <c r="D56" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E56" s="59"/>
     </row>
@@ -22078,13 +22075,13 @@
         <v>570</v>
       </c>
       <c r="B57" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C57">
         <v>90302117</v>
       </c>
       <c r="D57" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E57" s="59"/>
     </row>
@@ -22093,7 +22090,7 @@
         <v>570</v>
       </c>
       <c r="B58" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C58"/>
       <c r="D58" t="s">
@@ -22106,13 +22103,13 @@
         <v>570</v>
       </c>
       <c r="B59" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C59">
         <v>90300586</v>
       </c>
       <c r="D59" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E59" s="59"/>
     </row>
@@ -22121,13 +22118,13 @@
         <v>570</v>
       </c>
       <c r="B60" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C60">
         <v>90302487</v>
       </c>
       <c r="D60" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E60" s="59"/>
     </row>
@@ -22136,7 +22133,7 @@
         <v>570</v>
       </c>
       <c r="B61" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C61">
         <v>90302465</v>
@@ -22151,7 +22148,7 @@
         <v>570</v>
       </c>
       <c r="B62" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C62">
         <v>90117360</v>
@@ -22166,13 +22163,13 @@
         <v>570</v>
       </c>
       <c r="B63" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C63">
         <v>90302118</v>
       </c>
       <c r="D63" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E63" s="59"/>
     </row>
@@ -22181,13 +22178,13 @@
         <v>570</v>
       </c>
       <c r="B64" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C64">
         <v>90144804</v>
       </c>
       <c r="D64" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E64" s="59"/>
     </row>
@@ -22196,7 +22193,7 @@
         <v>570</v>
       </c>
       <c r="B65" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C65">
         <v>90302398</v>
@@ -22211,13 +22208,13 @@
         <v>570</v>
       </c>
       <c r="B66" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C66">
         <v>90302503</v>
       </c>
       <c r="D66" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E66" s="59"/>
     </row>
@@ -22226,13 +22223,13 @@
         <v>570</v>
       </c>
       <c r="B67" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C67">
         <v>90302504</v>
       </c>
       <c r="D67" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E67" s="59"/>
     </row>
@@ -22241,7 +22238,7 @@
         <v>570</v>
       </c>
       <c r="B68" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C68"/>
       <c r="D68" t="s">
@@ -22251,10 +22248,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B69" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C69">
         <v>90290068</v>
@@ -22269,16 +22266,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B70" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C70">
         <v>90302469</v>
       </c>
       <c r="D70" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E70" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
@@ -22287,16 +22284,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B71" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C71">
         <v>90302453</v>
       </c>
       <c r="D71" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E71" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
@@ -22305,16 +22302,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B72" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C72">
         <v>90301928</v>
       </c>
       <c r="D72" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E72" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
@@ -22323,16 +22320,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B73" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C73">
         <v>90302455</v>
       </c>
       <c r="D73" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E73" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
@@ -22341,10 +22338,10 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B74" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C74">
         <v>90302470</v>
@@ -22359,10 +22356,10 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B75" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C75">
         <v>90302471</v>
@@ -22377,16 +22374,16 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B76" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C76">
         <v>90302457</v>
       </c>
       <c r="D76" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E76" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
@@ -22395,14 +22392,14 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B77" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C77"/>
       <c r="D77" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E77" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
@@ -22411,16 +22408,16 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B78" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C78">
         <v>90290075</v>
       </c>
       <c r="D78" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E78" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
@@ -22429,16 +22426,16 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B79" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C79">
         <v>90302218</v>
       </c>
       <c r="D79" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E79" s="62" t="str">
         <f>IFERROR(VLOOKUP(#REF!,$G$2:$H$18,2,FALSE),"")</f>
@@ -22447,10 +22444,10 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B80" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C80">
         <v>90290074</v>
@@ -22465,10 +22462,10 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B81" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C81">
         <v>90301453</v>
@@ -22480,55 +22477,55 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B82" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C82">
         <v>90300620</v>
       </c>
       <c r="D82" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E82" s="62"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B83" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C83">
         <v>90290069</v>
       </c>
       <c r="D83" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E83" s="62"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B84" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C84">
         <v>90290077</v>
       </c>
       <c r="D84" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E84" s="62"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B85" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C85">
         <v>90301388</v>
@@ -22540,31 +22537,31 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B86" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C86">
         <v>90302500</v>
       </c>
       <c r="D86" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E86" s="62"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B87" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C87">
         <v>90302088</v>
       </c>
       <c r="D87" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E87" s="62" t="str">
         <f t="shared" ref="E87:E89" si="2">IFERROR(VLOOKUP(D87,$G$2:$H$18,2,FALSE),"")</f>
@@ -22573,16 +22570,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B88" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C88">
         <v>90302447</v>
       </c>
       <c r="D88" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E88" s="62" t="str">
         <f t="shared" si="2"/>
@@ -22591,12 +22588,12 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="60" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B89" s="61"/>
       <c r="C89"/>
       <c r="D89" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E89" s="62" t="str">
         <f t="shared" si="2"/>
@@ -22605,10 +22602,10 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="54" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B90" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C90">
         <v>90101732</v>
@@ -22619,38 +22616,38 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="54" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B91" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C91">
         <v>90302038</v>
       </c>
       <c r="D91" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="54" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B92" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C92">
         <v>90301852</v>
       </c>
       <c r="D92" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="54" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B93" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C93">
         <v>90128100</v>
@@ -22661,142 +22658,142 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="54" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B94" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C94">
         <v>90290053</v>
       </c>
       <c r="D94" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="54" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B95" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C95">
         <v>90300229</v>
       </c>
       <c r="D95" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="54" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B96" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C96">
         <v>90301651</v>
       </c>
       <c r="D96" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="54" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B97" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C97">
         <v>90302044</v>
       </c>
       <c r="D97" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="54" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B98" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C98">
         <v>90300312</v>
       </c>
       <c r="D98" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="54" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B99" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C99">
         <v>90300287</v>
       </c>
       <c r="D99" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="54" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B100" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C100">
         <v>90300546</v>
       </c>
       <c r="D100" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="54" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B101" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C101">
         <v>90300274</v>
       </c>
       <c r="D101" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="54" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B102" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C102">
         <v>90300281</v>
       </c>
       <c r="D102" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="60" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B103" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C103">
         <v>90302337</v>
       </c>
       <c r="D103" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -22854,8 +22851,8 @@
   </sheetPr>
   <dimension ref="A1:F397"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="G314" sqref="G314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22925,7 +22922,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>124</v>
       </c>
@@ -22942,7 +22939,7 @@
         <v>540</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -23023,7 +23020,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>124</v>
       </c>
@@ -23040,10 +23037,10 @@
         <v>540</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>125</v>
       </c>
@@ -23060,7 +23057,7 @@
         <v>540</v>
       </c>
       <c r="F10" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -23083,7 +23080,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>125</v>
       </c>
@@ -23100,10 +23097,10 @@
         <v>540</v>
       </c>
       <c r="F12" s="52" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>126</v>
       </c>
@@ -23120,7 +23117,7 @@
         <v>540</v>
       </c>
       <c r="F13" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -23183,7 +23180,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>126</v>
       </c>
@@ -23200,7 +23197,7 @@
         <v>540</v>
       </c>
       <c r="F17" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -23449,7 +23446,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>131</v>
       </c>
@@ -23466,7 +23463,7 @@
         <v>540</v>
       </c>
       <c r="F31" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -23509,7 +23506,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>131</v>
       </c>
@@ -23526,7 +23523,7 @@
         <v>540</v>
       </c>
       <c r="F34" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -23563,7 +23560,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>132</v>
       </c>
@@ -23580,7 +23577,7 @@
         <v>550</v>
       </c>
       <c r="F37" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -23617,7 +23614,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>134</v>
       </c>
@@ -23634,7 +23631,7 @@
         <v>550</v>
       </c>
       <c r="F40" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -23745,7 +23742,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>139</v>
       </c>
@@ -23762,7 +23759,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>139</v>
       </c>
@@ -23779,7 +23776,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>139</v>
       </c>
@@ -23796,7 +23793,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>139</v>
       </c>
@@ -23813,7 +23810,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>139</v>
       </c>
@@ -23830,7 +23827,7 @@
         <v>540</v>
       </c>
       <c r="F51" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -23927,7 +23924,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>139</v>
       </c>
@@ -23944,7 +23941,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>139</v>
       </c>
@@ -23961,7 +23958,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>139</v>
       </c>
@@ -23978,7 +23975,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>139</v>
       </c>
@@ -24035,7 +24032,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>139</v>
       </c>
@@ -24052,7 +24049,7 @@
         <v>540</v>
       </c>
       <c r="F63" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -24129,7 +24126,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>140</v>
       </c>
@@ -24146,7 +24143,7 @@
         <v>550</v>
       </c>
       <c r="F68" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -24598,7 +24595,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>146</v>
       </c>
@@ -24615,10 +24612,10 @@
         <v>540</v>
       </c>
       <c r="F94" s="52" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>146</v>
       </c>
@@ -24635,7 +24632,7 @@
         <v>540</v>
       </c>
       <c r="F95" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -24880,7 +24877,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>150</v>
       </c>
@@ -24897,7 +24894,7 @@
         <v>540</v>
       </c>
       <c r="F109" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -24977,7 +24974,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>150</v>
       </c>
@@ -24994,7 +24991,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>151</v>
       </c>
@@ -25011,7 +25008,7 @@
         <v>555</v>
       </c>
       <c r="F115" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -25367,7 +25364,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>160</v>
       </c>
@@ -25384,7 +25381,7 @@
         <v>540</v>
       </c>
       <c r="F135" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -25404,7 +25401,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>160</v>
       </c>
@@ -25421,7 +25418,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>160</v>
       </c>
@@ -25438,7 +25435,7 @@
         <v>550</v>
       </c>
       <c r="F138" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -25515,7 +25512,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>160</v>
       </c>
@@ -25532,7 +25529,7 @@
         <v>540</v>
       </c>
       <c r="F143" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -25655,7 +25652,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>164</v>
       </c>
@@ -25672,7 +25669,7 @@
         <v>540</v>
       </c>
       <c r="F150" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -25712,7 +25709,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>164</v>
       </c>
@@ -25729,7 +25726,7 @@
         <v>550</v>
       </c>
       <c r="F153" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -25749,7 +25746,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>164</v>
       </c>
@@ -25766,7 +25763,7 @@
         <v>540</v>
       </c>
       <c r="F155" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -25806,7 +25803,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>166</v>
       </c>
@@ -25823,7 +25820,7 @@
         <v>540</v>
       </c>
       <c r="F158" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -25843,7 +25840,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>166</v>
       </c>
@@ -25860,7 +25857,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>166</v>
       </c>
@@ -25877,7 +25874,7 @@
         <v>550</v>
       </c>
       <c r="F161" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -25897,7 +25894,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>166</v>
       </c>
@@ -25914,7 +25911,7 @@
         <v>540</v>
       </c>
       <c r="F163" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -25957,7 +25954,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>168</v>
       </c>
@@ -25974,10 +25971,10 @@
         <v>540</v>
       </c>
       <c r="F166" s="52" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>168</v>
       </c>
@@ -25994,7 +25991,7 @@
         <v>540</v>
       </c>
       <c r="F167" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -26014,7 +26011,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>168</v>
       </c>
@@ -26031,7 +26028,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
         <v>168</v>
       </c>
@@ -26048,7 +26045,7 @@
         <v>550</v>
       </c>
       <c r="F170" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -26125,7 +26122,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
         <v>168</v>
       </c>
@@ -26142,10 +26139,10 @@
         <v>540</v>
       </c>
       <c r="F175" s="52" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
         <v>168</v>
       </c>
@@ -26162,7 +26159,7 @@
         <v>540</v>
       </c>
       <c r="F176" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -26447,7 +26444,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
         <v>172</v>
       </c>
@@ -26464,7 +26461,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>172</v>
       </c>
@@ -26481,7 +26478,7 @@
         <v>550</v>
       </c>
       <c r="F193" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -26535,7 +26532,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
         <v>175</v>
       </c>
@@ -26552,10 +26549,10 @@
         <v>560</v>
       </c>
       <c r="F197" s="5" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
         <v>175</v>
       </c>
@@ -26572,10 +26569,10 @@
         <v>560</v>
       </c>
       <c r="F198" s="5" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
         <v>175</v>
       </c>
@@ -26592,7 +26589,7 @@
         <v>560</v>
       </c>
       <c r="F199" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -26669,7 +26666,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
         <v>175</v>
       </c>
@@ -26686,7 +26683,7 @@
         <v>560</v>
       </c>
       <c r="F204" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -26808,7 +26805,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
         <v>177</v>
       </c>
@@ -26825,7 +26822,7 @@
         <v>540</v>
       </c>
       <c r="F212" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -26987,7 +26984,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
         <v>177</v>
       </c>
@@ -27004,7 +27001,7 @@
         <v>550</v>
       </c>
       <c r="F222" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -27064,7 +27061,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
         <v>177</v>
       </c>
@@ -27081,10 +27078,10 @@
         <v>540</v>
       </c>
       <c r="F226" s="52" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="5" t="s">
         <v>178</v>
       </c>
@@ -27101,7 +27098,7 @@
         <v>540</v>
       </c>
       <c r="F227" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -27172,7 +27169,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="5" t="s">
         <v>178</v>
       </c>
@@ -27189,7 +27186,7 @@
         <v>550</v>
       </c>
       <c r="F232" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -27693,7 +27690,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="260" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="5" t="s">
         <v>185</v>
       </c>
@@ -27710,7 +27707,7 @@
         <v>550</v>
       </c>
       <c r="F260" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="261" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -27753,7 +27750,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="5" t="s">
         <v>185</v>
       </c>
@@ -27770,10 +27767,10 @@
         <v>551</v>
       </c>
       <c r="F263" s="5" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="264" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="5" t="s">
         <v>185</v>
       </c>
@@ -27790,7 +27787,7 @@
         <v>540</v>
       </c>
       <c r="F264" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="265" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -27924,7 +27921,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="272" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="5" t="s">
         <v>185</v>
       </c>
@@ -27941,7 +27938,7 @@
         <v>550</v>
       </c>
       <c r="F272" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="273" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -27964,7 +27961,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="5" t="s">
         <v>185</v>
       </c>
@@ -27981,7 +27978,7 @@
         <v>551</v>
       </c>
       <c r="F274" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="275" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -28024,7 +28021,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="277" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" s="5" t="s">
         <v>185</v>
       </c>
@@ -28041,7 +28038,7 @@
         <v>540</v>
       </c>
       <c r="F277" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="278" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -28175,7 +28172,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="285" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" s="5" t="s">
         <v>188</v>
       </c>
@@ -28192,7 +28189,7 @@
         <v>540</v>
       </c>
       <c r="F285" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="286" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -28232,7 +28229,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="288" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="5" t="s">
         <v>188</v>
       </c>
@@ -28249,7 +28246,7 @@
         <v>550</v>
       </c>
       <c r="F288" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="289" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -28269,7 +28266,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="290" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" s="5" t="s">
         <v>188</v>
       </c>
@@ -28286,7 +28283,7 @@
         <v>540</v>
       </c>
       <c r="F290" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="291" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -28394,7 +28391,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="297" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" s="5" t="s">
         <v>193</v>
       </c>
@@ -28411,7 +28408,7 @@
         <v>540</v>
       </c>
       <c r="F297" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="298" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -28451,7 +28448,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="300" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" s="5" t="s">
         <v>193</v>
       </c>
@@ -28468,7 +28465,7 @@
         <v>550</v>
       </c>
       <c r="F300" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="301" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -28545,7 +28542,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="305" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="5" t="s">
         <v>193</v>
       </c>
@@ -28562,7 +28559,7 @@
         <v>540</v>
       </c>
       <c r="F305" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="306" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -28585,7 +28582,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="307" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" s="5" t="s">
         <v>194</v>
       </c>
@@ -28602,7 +28599,7 @@
         <v>540</v>
       </c>
       <c r="F307" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="308" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -28642,7 +28639,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="310" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310" s="5" t="s">
         <v>194</v>
       </c>
@@ -28659,7 +28656,7 @@
         <v>550</v>
       </c>
       <c r="F310" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="311" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -28679,7 +28676,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="312" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312" s="5" t="s">
         <v>194</v>
       </c>
@@ -28696,7 +28693,7 @@
         <v>540</v>
       </c>
       <c r="F312" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="313" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -28719,7 +28716,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="314" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A314" s="5" t="s">
         <v>195</v>
       </c>
@@ -28736,10 +28733,10 @@
         <v>540</v>
       </c>
       <c r="F314" s="52" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="315" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A315" s="5" t="s">
         <v>195</v>
       </c>
@@ -28756,7 +28753,7 @@
         <v>540</v>
       </c>
       <c r="F315" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="316" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -28796,7 +28793,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="318" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" s="5" t="s">
         <v>195</v>
       </c>
@@ -28813,7 +28810,7 @@
         <v>550</v>
       </c>
       <c r="F318" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="319" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -28890,7 +28887,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="323" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A323" s="5" t="s">
         <v>195</v>
       </c>
@@ -28907,10 +28904,10 @@
         <v>540</v>
       </c>
       <c r="F323" s="52" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="324" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A324" s="5" t="s">
         <v>195</v>
       </c>
@@ -28927,7 +28924,7 @@
         <v>540</v>
       </c>
       <c r="F324" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="325" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -29110,7 +29107,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="334" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A334" s="5" t="s">
         <v>203</v>
       </c>
@@ -29127,7 +29124,7 @@
         <v>540</v>
       </c>
       <c r="F334" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="335" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -29227,7 +29224,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" s="5" t="s">
         <v>203</v>
       </c>
@@ -29244,7 +29241,7 @@
         <v>551</v>
       </c>
       <c r="F340" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="341" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -29421,7 +29418,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="350" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A350" s="5" t="s">
         <v>207</v>
       </c>
@@ -29438,7 +29435,7 @@
         <v>550</v>
       </c>
       <c r="F350" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="351" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -29475,7 +29472,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="353" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A353" s="5" t="s">
         <v>209</v>
       </c>
@@ -29492,10 +29489,10 @@
         <v>567</v>
       </c>
       <c r="F353" s="52" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="354" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A354" s="5" t="s">
         <v>209</v>
       </c>
@@ -29512,10 +29509,10 @@
         <v>540</v>
       </c>
       <c r="F354" s="52" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" s="5" t="s">
         <v>210</v>
       </c>
@@ -29532,10 +29529,10 @@
         <v>560</v>
       </c>
       <c r="F355" s="5" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" s="5" t="s">
         <v>210</v>
       </c>
@@ -29552,10 +29549,10 @@
         <v>560</v>
       </c>
       <c r="F356" s="5" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" s="5" t="s">
         <v>210</v>
       </c>
@@ -29572,10 +29569,10 @@
         <v>560</v>
       </c>
       <c r="F357" s="5" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" s="5" t="s">
         <v>210</v>
       </c>
@@ -29592,7 +29589,7 @@
         <v>560</v>
       </c>
       <c r="F358" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="359" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -29669,7 +29666,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" s="5" t="s">
         <v>210</v>
       </c>
@@ -29686,10 +29683,10 @@
         <v>560</v>
       </c>
       <c r="F363" s="5" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" s="5" t="s">
         <v>210</v>
       </c>
@@ -29706,7 +29703,7 @@
         <v>560</v>
       </c>
       <c r="F364" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="365" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -29763,7 +29760,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" s="5" t="s">
         <v>211</v>
       </c>
@@ -29780,10 +29777,10 @@
         <v>560</v>
       </c>
       <c r="F368" s="5" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" s="5" t="s">
         <v>211</v>
       </c>
@@ -29800,10 +29797,10 @@
         <v>560</v>
       </c>
       <c r="F369" s="5" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" s="5" t="s">
         <v>211</v>
       </c>
@@ -29820,7 +29817,7 @@
         <v>560</v>
       </c>
       <c r="F370" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="371" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -29897,7 +29894,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" s="5" t="s">
         <v>211</v>
       </c>
@@ -29914,7 +29911,7 @@
         <v>560</v>
       </c>
       <c r="F375" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="376" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -29934,7 +29931,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" s="5" t="s">
         <v>211</v>
       </c>
@@ -29951,7 +29948,7 @@
         <v>560</v>
       </c>
       <c r="F377" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="378" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -30156,7 +30153,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="389" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A389" s="5" t="s">
         <v>217</v>
       </c>
@@ -30173,7 +30170,7 @@
         <v>555</v>
       </c>
       <c r="F389" s="52" t="s">
-        <v>571</v>
+        <v>644</v>
       </c>
     </row>
     <row r="390" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -30329,10 +30326,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F397" xr:uid="{3928BC1A-32B2-4777-AAB5-998C660AF0A9}">
-    <filterColumn colId="4">
+    <filterColumn colId="5">
       <filters>
-        <filter val="000SWCS"/>
-        <filter val="000SWME"/>
+        <filter val="SMS"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -30341,15 +30337,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004A5BF6C7F67B434096FAC9443A83D821" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1347de4a6797875f8d6b1ac5dc93737c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d41b7399-51ed-4fce-9e89-79a41c55ed41" xmlns:ns3="a1bbf4fc-2070-4842-8cf2-c42346818ea9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="67ec082bb3101a8db1bb88f037f675cb" ns2:_="" ns3:_="">
     <xsd:import namespace="d41b7399-51ed-4fce-9e89-79a41c55ed41"/>
@@ -30592,6 +30579,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -30604,14 +30600,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71C3BF75-E265-495B-A1EF-9F0F8014FF62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F00606B-6B80-42B0-B0DE-C79F0839CF7D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -30630,6 +30618,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71C3BF75-E265-495B-A1EF-9F0F8014FF62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C286B8F-44DD-46A1-8664-5B3AFC40D364}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
update Crane Driver title
</commit_message>
<xml_diff>
--- a/public/data/Master App Timesheet.xlsx
+++ b/public/data/Master App Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\timesheet-app\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047916CC-BCC6-48B0-9AB8-2A18B2050BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7425D95D-C052-41A4-BE77-31376118CC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2871" uniqueCount="675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2871" uniqueCount="673">
   <si>
     <t xml:space="preserve">Date
 </t>
@@ -1992,24 +1992,12 @@
     <t>TMS Boilermaker</t>
   </si>
   <si>
-    <t xml:space="preserve">Boom Crane Operator </t>
-  </si>
-  <si>
     <t>Boom Rigger</t>
   </si>
   <si>
     <t>Boom Supervisor</t>
   </si>
   <si>
-    <t>Boom Crane Op 320T</t>
-  </si>
-  <si>
-    <t>Boom Crane Op 70T</t>
-  </si>
-  <si>
-    <t>Boom Crane Op 160T</t>
-  </si>
-  <si>
     <t>GMRS Supervisor</t>
   </si>
   <si>
@@ -2122,6 +2110,12 @@
   </si>
   <si>
     <t>Chloe Cameron</t>
+  </si>
+  <si>
+    <t>Crane Operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crane Operator </t>
   </si>
 </sst>
 </file>
@@ -22190,7 +22184,7 @@
   <dimension ref="A1:L101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22250,13 +22244,13 @@
         <v>90140920</v>
       </c>
       <c r="D2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="E2" s="21">
         <v>3001951</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>631</v>
+        <v>672</v>
       </c>
       <c r="H2" s="21">
         <v>3001951</v>
@@ -22276,19 +22270,19 @@
         <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="C3">
         <v>90301465</v>
       </c>
       <c r="D3" t="s">
-        <v>634</v>
+        <v>671</v>
       </c>
       <c r="E3" s="21">
         <v>3001951</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="H3" s="21">
         <v>3001951</v>
@@ -22308,7 +22302,7 @@
       <c r="C4"/>
       <c r="E4" s="21"/>
       <c r="G4" s="11" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="H4" s="21">
         <v>3001951</v>
@@ -22333,8 +22327,8 @@
       <c r="C5">
         <v>90300849</v>
       </c>
-      <c r="D5" t="s">
-        <v>632</v>
+      <c r="D5" s="11" t="s">
+        <v>631</v>
       </c>
       <c r="E5" s="21">
         <v>3001951</v>
@@ -22360,13 +22354,13 @@
         <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="C6">
         <v>90302562</v>
       </c>
-      <c r="D6" t="s">
-        <v>632</v>
+      <c r="D6" s="11" t="s">
+        <v>631</v>
       </c>
       <c r="E6" s="21">
         <v>3001951</v>
@@ -22392,13 +22386,13 @@
         <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C7">
         <v>90302563</v>
       </c>
       <c r="D7" t="s">
-        <v>635</v>
+        <v>671</v>
       </c>
       <c r="E7" s="21">
         <v>3001951</v>
@@ -22429,14 +22423,14 @@
       <c r="C8">
         <v>90300016</v>
       </c>
-      <c r="D8" t="s">
-        <v>632</v>
+      <c r="D8" s="11" t="s">
+        <v>631</v>
       </c>
       <c r="E8" s="21">
         <v>3001951</v>
       </c>
       <c r="G8" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="H8" s="11">
         <v>3001951</v>
@@ -22453,13 +22447,13 @@
         <v>90301850</v>
       </c>
       <c r="D9" t="s">
-        <v>636</v>
+        <v>671</v>
       </c>
       <c r="E9" s="21">
         <v>3001951</v>
       </c>
       <c r="G9" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H9" s="11">
         <v>3001951</v>
@@ -22475,14 +22469,14 @@
       <c r="C10">
         <v>90302512</v>
       </c>
-      <c r="D10" t="s">
-        <v>632</v>
+      <c r="D10" s="11" t="s">
+        <v>631</v>
       </c>
       <c r="E10" s="21">
         <v>3001951</v>
       </c>
       <c r="G10" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="H10" s="11">
         <v>3001951</v>
@@ -22499,13 +22493,13 @@
         <v>90137237</v>
       </c>
       <c r="D11" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="E11" s="21">
         <v>3001951</v>
       </c>
       <c r="G11" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="H11" s="11">
         <v>3001951</v>
@@ -22522,13 +22516,13 @@
         <v>90300199</v>
       </c>
       <c r="D12" t="s">
-        <v>634</v>
+        <v>671</v>
       </c>
       <c r="E12" s="21">
         <v>3001951</v>
       </c>
       <c r="G12" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="H12" s="11">
         <v>3001951</v>
@@ -22544,14 +22538,14 @@
       <c r="C13">
         <v>90300019</v>
       </c>
-      <c r="D13" t="s">
-        <v>632</v>
+      <c r="D13" s="11" t="s">
+        <v>631</v>
       </c>
       <c r="E13" s="21">
         <v>3001951</v>
       </c>
       <c r="G13" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="H13" s="11">
         <v>3001951</v>
@@ -22567,14 +22561,14 @@
       <c r="C14">
         <v>90301314</v>
       </c>
-      <c r="D14" t="s">
-        <v>632</v>
+      <c r="D14" s="11" t="s">
+        <v>631</v>
       </c>
       <c r="E14" s="21">
         <v>3001951</v>
       </c>
       <c r="G14" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="H14" s="11">
         <v>3001951</v>
@@ -22591,13 +22585,13 @@
         <v>90302329</v>
       </c>
       <c r="D15" t="s">
-        <v>635</v>
+        <v>671</v>
       </c>
       <c r="E15" s="21">
         <v>3001951</v>
       </c>
       <c r="G15" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="H15" s="11">
         <v>3001951</v>
@@ -22613,14 +22607,14 @@
       <c r="C16">
         <v>90300213</v>
       </c>
-      <c r="D16" t="s">
-        <v>632</v>
+      <c r="D16" s="11" t="s">
+        <v>631</v>
       </c>
       <c r="E16" s="21">
         <v>3001951</v>
       </c>
       <c r="G16" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="H16" s="11">
         <v>3001951</v>
@@ -22637,13 +22631,13 @@
         <v>90301259</v>
       </c>
       <c r="D17" t="s">
-        <v>636</v>
+        <v>671</v>
       </c>
       <c r="E17" s="21">
         <v>3001951</v>
       </c>
       <c r="G17" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="H17" s="11">
         <v>3001951</v>
@@ -22659,14 +22653,14 @@
       <c r="C18">
         <v>90300214</v>
       </c>
-      <c r="D18" t="s">
-        <v>632</v>
+      <c r="D18" s="11" t="s">
+        <v>631</v>
       </c>
       <c r="E18" s="21">
         <v>3001951</v>
       </c>
       <c r="G18" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="H18" s="11">
         <v>3001951</v>
@@ -22677,19 +22671,19 @@
         <v>567</v>
       </c>
       <c r="B19" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="C19">
         <v>90300498</v>
       </c>
       <c r="D19" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="E19" s="21">
         <v>3001951</v>
       </c>
       <c r="G19" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="H19" s="11">
         <v>3001951</v>
@@ -22700,19 +22694,19 @@
         <v>567</v>
       </c>
       <c r="B20" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="C20">
         <v>90302549</v>
       </c>
       <c r="D20" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="E20" s="21">
         <v>3001951</v>
       </c>
       <c r="G20" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="H20" s="11">
         <v>3001951</v>
@@ -22723,13 +22717,13 @@
         <v>567</v>
       </c>
       <c r="B21" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="C21">
         <v>90302546</v>
       </c>
       <c r="D21" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="E21" s="21">
         <v>3001951</v>
@@ -22747,7 +22741,7 @@
         <v>90300003</v>
       </c>
       <c r="D22" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="E22" s="21">
         <v>3001951</v>
@@ -22764,7 +22758,7 @@
         <v>90302529</v>
       </c>
       <c r="D23" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="E23" s="21">
         <v>3001951</v>
@@ -22781,7 +22775,7 @@
         <v>90300039</v>
       </c>
       <c r="D24" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="E24" s="21">
         <v>3001951</v>
@@ -22798,7 +22792,7 @@
         <v>90144128</v>
       </c>
       <c r="D25" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="E25" s="21">
         <v>3001951</v>
@@ -22809,13 +22803,13 @@
         <v>567</v>
       </c>
       <c r="B26" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="C26">
         <v>90302547</v>
       </c>
       <c r="D26" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="E26" s="21">
         <v>3001951</v>
@@ -22832,7 +22826,7 @@
         <v>90301392</v>
       </c>
       <c r="D27" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="E27" s="21">
         <v>3001951</v>
@@ -22843,13 +22837,13 @@
         <v>567</v>
       </c>
       <c r="B28" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="C28">
         <v>90302551</v>
       </c>
       <c r="D28" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="E28" s="21">
         <v>3001951</v>
@@ -22894,7 +22888,7 @@
         <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="C31">
         <v>90302553</v>
@@ -22945,7 +22939,7 @@
         <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="C34">
         <v>90301904</v>
@@ -23064,7 +23058,7 @@
         <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="C41">
         <v>90301210</v>
@@ -23098,13 +23092,13 @@
         <v>568</v>
       </c>
       <c r="B43" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="C43">
         <v>90116535</v>
       </c>
       <c r="D43" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="E43" s="50"/>
     </row>
@@ -23119,7 +23113,7 @@
         <v>90300462</v>
       </c>
       <c r="D44" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="E44" s="50"/>
     </row>
@@ -23134,7 +23128,7 @@
         <v>90302117</v>
       </c>
       <c r="D45" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="E45" s="50"/>
     </row>
@@ -23149,7 +23143,7 @@
         <v>90302543</v>
       </c>
       <c r="D46" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="E46" s="50"/>
     </row>
@@ -23158,13 +23152,13 @@
         <v>568</v>
       </c>
       <c r="B47" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="C47">
         <v>90302565</v>
       </c>
       <c r="D47" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="E47" s="50"/>
     </row>
@@ -23180,13 +23174,13 @@
         <v>568</v>
       </c>
       <c r="B49" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="C49">
         <v>90137959</v>
       </c>
       <c r="D49" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="E49" s="50"/>
     </row>
@@ -23216,7 +23210,7 @@
         <v>90302118</v>
       </c>
       <c r="D51" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="E51" s="50"/>
     </row>
@@ -23231,7 +23225,7 @@
         <v>90144804</v>
       </c>
       <c r="D52" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="E52" s="50"/>
     </row>
@@ -23246,7 +23240,7 @@
         <v>90302398</v>
       </c>
       <c r="D53" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="E53" s="50"/>
     </row>
@@ -23255,13 +23249,13 @@
         <v>568</v>
       </c>
       <c r="B54" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="C54">
         <v>90302559</v>
       </c>
       <c r="D54" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="E54" s="50"/>
     </row>
@@ -23276,7 +23270,7 @@
         <v>90302504</v>
       </c>
       <c r="D55" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="E55" s="50"/>
     </row>
@@ -23291,7 +23285,7 @@
         <v>90302527</v>
       </c>
       <c r="D56" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -23305,7 +23299,7 @@
         <v>90290068</v>
       </c>
       <c r="D57" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -23319,7 +23313,7 @@
         <v>90302469</v>
       </c>
       <c r="D58" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -23327,13 +23321,13 @@
         <v>569</v>
       </c>
       <c r="B59" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="C59">
         <v>90302531</v>
       </c>
       <c r="D59" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -23347,7 +23341,7 @@
         <v>90301928</v>
       </c>
       <c r="D60" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -23375,7 +23369,7 @@
         <v>90302470</v>
       </c>
       <c r="D62" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -23383,7 +23377,7 @@
         <v>569</v>
       </c>
       <c r="B63" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="C63">
         <v>90302463</v>
@@ -23403,7 +23397,7 @@
         <v>90302457</v>
       </c>
       <c r="D64" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -23411,13 +23405,13 @@
         <v>569</v>
       </c>
       <c r="B65" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="C65">
         <v>90290070</v>
       </c>
       <c r="D65" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -23431,7 +23425,7 @@
         <v>90290075</v>
       </c>
       <c r="D66" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -23445,7 +23439,7 @@
         <v>90302218</v>
       </c>
       <c r="D67" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -23459,7 +23453,7 @@
         <v>90290074</v>
       </c>
       <c r="D68" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -23467,11 +23461,11 @@
         <v>606</v>
       </c>
       <c r="B69" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="C69"/>
       <c r="D69" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -23479,13 +23473,13 @@
         <v>606</v>
       </c>
       <c r="B70" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="C70">
         <v>90137312</v>
       </c>
       <c r="D70" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -23499,7 +23493,7 @@
         <v>90301852</v>
       </c>
       <c r="D71" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -23513,7 +23507,7 @@
         <v>90128100</v>
       </c>
       <c r="D72" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -23527,7 +23521,7 @@
         <v>90290053</v>
       </c>
       <c r="D73" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -23535,13 +23529,13 @@
         <v>606</v>
       </c>
       <c r="B74" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="C74">
         <v>90301507</v>
       </c>
       <c r="D74" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -23555,7 +23549,7 @@
         <v>90301651</v>
       </c>
       <c r="D75" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -23569,7 +23563,7 @@
         <v>90302044</v>
       </c>
       <c r="D76" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -23583,7 +23577,7 @@
         <v>90300312</v>
       </c>
       <c r="D77" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -23591,13 +23585,13 @@
         <v>606</v>
       </c>
       <c r="B78" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="C78">
         <v>90300287</v>
       </c>
       <c r="D78" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -23611,7 +23605,7 @@
         <v>90300546</v>
       </c>
       <c r="D79" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -23625,7 +23619,7 @@
         <v>90300274</v>
       </c>
       <c r="D80" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -23639,7 +23633,7 @@
         <v>90300281</v>
       </c>
       <c r="D81" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -23647,13 +23641,13 @@
         <v>606</v>
       </c>
       <c r="B82" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C82">
         <v>90300273</v>
       </c>
       <c r="D82" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -31191,6 +31185,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a1bbf4fc-2070-4842-8cf2-c42346818ea9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d41b7399-51ed-4fce-9e89-79a41c55ed41">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004A5BF6C7F67B434096FAC9443A83D821" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1347de4a6797875f8d6b1ac5dc93737c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d41b7399-51ed-4fce-9e89-79a41c55ed41" xmlns:ns3="a1bbf4fc-2070-4842-8cf2-c42346818ea9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="67ec082bb3101a8db1bb88f037f675cb" ns2:_="" ns3:_="">
     <xsd:import namespace="d41b7399-51ed-4fce-9e89-79a41c55ed41"/>
@@ -31433,27 +31447,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a1bbf4fc-2070-4842-8cf2-c42346818ea9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d41b7399-51ed-4fce-9e89-79a41c55ed41">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71C3BF75-E265-495B-A1EF-9F0F8014FF62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C286B8F-44DD-46A1-8664-5B3AFC40D364}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a1bbf4fc-2070-4842-8cf2-c42346818ea9"/>
+    <ds:schemaRef ds:uri="d41b7399-51ed-4fce-9e89-79a41c55ed41"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F00606B-6B80-42B0-B0DE-C79F0839CF7D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -31470,23 +31483,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C286B8F-44DD-46A1-8664-5B3AFC40D364}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a1bbf4fc-2070-4842-8cf2-c42346818ea9"/>
-    <ds:schemaRef ds:uri="d41b7399-51ed-4fce-9e89-79a41c55ed41"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71C3BF75-E265-495B-A1EF-9F0F8014FF62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>